<commit_message>
docs: clean up content in K-Means.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{096302A2-9E9B-C441-B8B7-8198272E8146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB41C974-A70B-814E-9B19-CADB6923098D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56120" yWindow="6200" windowWidth="27640" windowHeight="15580" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
   <si>
     <t>Topic</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Multivariate Distributions</t>
+  </si>
+  <si>
+    <t>Voronoi Region</t>
   </si>
 </sst>
 </file>
@@ -458,13 +461,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -790,11 +794,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1007,30 +1011,28 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
+      <c r="A7" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3">
-        <v>8.1</v>
-      </c>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1044,7 +1046,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3">
-        <v>8.1999999999999993</v>
+        <v>8.1</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1052,7 +1054,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1063,12 +1065,10 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3">
-        <v>17</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1087,10 +1087,12 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3">
+        <v>17</v>
+      </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3">
-        <v>8.4</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1098,25 +1100,21 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J11" s="3">
-        <v>17.3</v>
-      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="3">
-        <v>7.1</v>
+        <v>8.4</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1124,7 +1122,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1135,12 +1133,14 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="J12" s="3">
-        <v>17.2</v>
+        <v>17.3</v>
       </c>
       <c r="K12" s="3">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1161,10 +1161,10 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3">
-        <v>17</v>
+        <v>17.2</v>
       </c>
       <c r="K13" s="3">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1172,28 +1172,23 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>40</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>45</v>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>17</v>
       </c>
       <c r="K14" s="3">
-        <v>3.1</v>
+        <v>6</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1201,7 +1196,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>18</v>
@@ -1209,6 +1204,7 @@
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
         <v>44</v>
@@ -1216,10 +1212,10 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="J15" s="3">
-        <v>11.3</v>
+        <v>3.2</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="K15" s="3">
         <v>3.1</v>
@@ -1230,7 +1226,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
@@ -1238,6 +1234,7 @@
       <c r="C16" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
         <v>44</v>
@@ -1248,7 +1245,7 @@
         <v>3.4</v>
       </c>
       <c r="J16" s="3">
-        <v>11.4</v>
+        <v>11.3</v>
       </c>
       <c r="K16" s="3">
         <v>3.1</v>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
@@ -1267,18 +1264,21 @@
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
         <v>44</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <v>3.4</v>
+      </c>
       <c r="J17" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>49</v>
+        <v>11.4</v>
+      </c>
+      <c r="K17" s="3">
+        <v>3.1</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>18</v>
@@ -1294,26 +1294,27 @@
       <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>18</v>
@@ -1321,6 +1322,7 @@
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
         <v>19</v>
@@ -1340,7 +1342,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -1348,30 +1350,27 @@
       <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>18</v>
@@ -1382,19 +1381,20 @@
       <c r="D21" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.5</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>18</v>
@@ -1413,15 +1413,20 @@
       <c r="D22" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="K22" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1429,13 +1434,16 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
@@ -1444,11 +1452,9 @@
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="3">
-        <v>10.5</v>
-      </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>18</v>
@@ -1464,55 +1470,58 @@
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3">
-        <v>12</v>
-      </c>
-      <c r="K24" s="3"/>
+        <v>10.5</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="3">
-        <v>13.3</v>
-      </c>
+      <c r="I25" s="3"/>
       <c r="J25" s="3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>67</v>
       </c>
@@ -1521,46 +1530,48 @@
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3">
+        <v>13.4</v>
+      </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="3">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>71</v>
@@ -1568,12 +1579,10 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3">
-        <v>8.5</v>
-      </c>
+      <c r="I28" s="3"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="3" t="s">
-        <v>72</v>
+      <c r="K28" s="3">
+        <v>9.1999999999999993</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1581,33 +1590,33 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="I29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3">
+        <v>8.5</v>
+      </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="K29" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>22</v>
@@ -1620,96 +1629,92 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="N30" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3">
+        <v>6.4</v>
+      </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="3">
-        <v>16.2</v>
-      </c>
+      <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="I32" s="3"/>
       <c r="J32" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>16.2</v>
+      </c>
+      <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="N32" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3">
-        <v>9.1999999999999993</v>
+      <c r="I33" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="J33" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="K33" s="3">
-        <v>14.4</v>
+        <v>16.3</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1717,31 +1722,37 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D34" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
-        <v>8.6999999999999993</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="J34" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="K34" s="3"/>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="K34" s="3">
+        <v>14.4</v>
+      </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1753,21 +1764,19 @@
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
-        <v>8.8000000000000007</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J35" s="3">
-        <v>18.2</v>
-      </c>
-      <c r="K35" s="3">
-        <v>14.1</v>
-      </c>
+        <v>18.3</v>
+      </c>
+      <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1779,19 +1788,21 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
-        <v>15</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J36" s="3">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="K36" s="3"/>
+        <v>18.2</v>
+      </c>
+      <c r="K36" s="3">
+        <v>14.1</v>
+      </c>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1803,10 +1814,10 @@
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J37" s="3">
-        <v>18.5</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -1815,20 +1826,22 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3">
+        <v>16</v>
+      </c>
       <c r="J38" s="3">
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -1837,7 +1850,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1859,7 +1872,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1881,7 +1894,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1903,7 +1916,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1925,7 +1938,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1947,7 +1960,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1969,24 +1982,20 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="3">
-        <v>14.5</v>
-      </c>
+      <c r="I45" s="3"/>
       <c r="J45" s="3">
-        <v>20.100000000000001</v>
+        <v>19</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -1995,7 +2004,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>32</v>
@@ -2008,9 +2017,11 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="I46" s="3">
+        <v>14.5</v>
+      </c>
       <c r="J46" s="3">
-        <v>20.2</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -2019,7 +2030,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>32</v>
@@ -2034,7 +2045,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="J47" s="3">
-        <v>20.3</v>
+        <v>20.2</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2043,7 +2054,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>32</v>
@@ -2058,7 +2069,7 @@
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
       <c r="J48" s="3">
-        <v>20.399999999999999</v>
+        <v>20.3</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
@@ -2067,7 +2078,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>32</v>
@@ -2082,7 +2093,7 @@
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
       <c r="J49" s="3">
-        <v>20.5</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -2091,24 +2102,22 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3">
-        <v>21.5</v>
+        <v>20.5</v>
       </c>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -2117,7 +2126,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>32</v>
@@ -2134,7 +2143,7 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3">
-        <v>21.4</v>
+        <v>21.5</v>
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2143,35 +2152,37 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="D52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3">
-        <v>20.5</v>
+        <v>21.4</v>
       </c>
       <c r="K52" s="3"/>
-      <c r="L52" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="M52" s="3">
-        <v>6.8</v>
-      </c>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
       <c r="N52" s="3"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2179,15 +2190,21 @@
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="3">
+        <v>20.5</v>
+      </c>
       <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
+      <c r="L53" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="M53" s="3">
+        <v>6.8</v>
+      </c>
       <c r="N53" s="3"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -2199,15 +2216,13 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
-      <c r="L54" s="3">
-        <v>9</v>
-      </c>
+      <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -2220,14 +2235,14 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -2247,15 +2262,11 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="3"/>
-      <c r="C57" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2263,13 +2274,15 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
+      <c r="L57" s="3">
+        <v>10</v>
+      </c>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B58" s="3"/>
       <c r="C58" s="3" t="s">
@@ -2291,7 +2304,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B59" s="3"/>
       <c r="C59" s="3" t="s">
@@ -2313,7 +2326,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3" t="s">
@@ -2335,14 +2348,14 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -2357,7 +2370,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3" t="s">
@@ -2379,7 +2392,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3" t="s">
@@ -2401,11 +2414,11 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>116</v>
@@ -2421,9 +2434,34 @@
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
     </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N64" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <conditionalFormatting sqref="A2:N13 A25:N64 A14:C24 E14:N19 E23:N24 F20:N22 D20:D22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N65">
+    <sortCondition ref="G2:G65"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:N13 A25:N64 A14:C24 E14:N19 E23:N24 F20:N22 D20:D22 A65">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2="Completed"</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: clean up K-Means content and start on Gaussian Mixtures.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB41C974-A70B-814E-9B19-CADB6923098D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEA9EA9-69A7-5049-B025-D5BCB1154F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="56120" yWindow="6200" windowWidth="27640" windowHeight="15580" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="123">
   <si>
     <t>Topic</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Voronoi Region</t>
+  </si>
+  <si>
+    <t>Mixtures</t>
   </si>
 </sst>
 </file>
@@ -461,14 +464,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,8 +799,8 @@
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1011,7 +1013,7 @@
       <c r="N6" s="2"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B7" s="3"/>
@@ -1569,7 +1571,9 @@
         <v>70</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
migrate: migrate my optimization notes to this repo.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEA9EA9-69A7-5049-B025-D5BCB1154F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5DB18-BEE7-F14B-BD8E-4837EAFD50E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56120" yWindow="6200" windowWidth="27640" windowHeight="15580" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
+    <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$N$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$71</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="133">
   <si>
     <t>Topic</t>
   </si>
@@ -408,6 +408,36 @@
   </si>
   <si>
     <t>Mixtures</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Concept</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Image compression and segmentation.</t>
+  </si>
+  <si>
+    <t>Non-vectorized K-Means implementation.</t>
+  </si>
+  <si>
+    <t>Gradient Descent</t>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Consider linking logistic regression's implementation to here.</t>
   </si>
 </sst>
 </file>
@@ -437,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -460,17 +490,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,11 +872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -811,14 +887,15 @@
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="97.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="97.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,32 +915,35 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -882,529 +962,501 @@
         <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
         <v>4.2</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>4.2</v>
       </c>
-      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" s="2">
-        <v>6.2</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2">
+        <v>6.2</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
-        <v>33</v>
-      </c>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2">
-        <v>9.1</v>
-      </c>
+      <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3">
-        <v>17</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3">
-        <v>8.4</v>
-      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>39</v>
+      <c r="O11" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="C12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="3">
-        <v>17.3</v>
-      </c>
-      <c r="K12" s="3">
-        <v>7.1</v>
-      </c>
+      <c r="G12" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="C13" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3">
-        <v>17.2</v>
-      </c>
-      <c r="K13" s="3">
-        <v>6.4</v>
-      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="C14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3">
-        <v>17</v>
-      </c>
-      <c r="K14" s="3">
-        <v>6</v>
-      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="L15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3">
+        <v>8.1</v>
+      </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="J16" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="K16" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="L16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3">
-        <v>3.4</v>
-      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="3">
-        <v>11.4</v>
-      </c>
-      <c r="K17" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="L17" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
+        <v>8.4</v>
+      </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3">
-        <v>4.3</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="K19" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L19" s="3">
+        <v>7.1</v>
+      </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="L20" s="3">
+        <v>6.4</v>
+      </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3">
+        <v>17</v>
+      </c>
+      <c r="L21" s="3">
+        <v>6</v>
+      </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>18</v>
@@ -1412,31 +1464,30 @@
       <c r="C22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>58</v>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <v>3.2</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L22" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="L22" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>18</v>
@@ -1444,27 +1495,30 @@
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" s="3"/>
+      <c r="J23" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="K23" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="L23" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>18</v>
@@ -1475,24 +1529,27 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="L24" s="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="K24" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="L24" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>18</v>
@@ -1502,430 +1559,487 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3">
-        <v>12</v>
-      </c>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="3">
-        <v>13.3</v>
-      </c>
+      <c r="I26" s="3"/>
       <c r="J26" s="3">
-        <v>16.100000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C28" s="3" t="s">
-        <v>122</v>
+        <v>16</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="L28" s="3"/>
+      <c r="J28" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F29" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="J29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3">
+        <v>4.4000000000000004</v>
+      </c>
       <c r="K29" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L29" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D30" s="3" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="3">
-        <v>6.3</v>
-      </c>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="L30" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="M30" s="3"/>
-      <c r="N30" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3">
-        <v>6.4</v>
-      </c>
+      <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="K31" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C32" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>76</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="K32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3">
+        <v>12</v>
+      </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="I33" s="3"/>
       <c r="J33" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L33" s="3"/>
+        <v>13.3</v>
+      </c>
+      <c r="K33" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="I34" s="3"/>
       <c r="J34" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="K34" s="3">
-        <v>14.4</v>
-      </c>
+        <v>13.4</v>
+      </c>
+      <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="C35" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D35" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="J35" s="3">
-        <v>18.3</v>
-      </c>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="L35" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="3">
-        <v>8.8000000000000007</v>
-      </c>
+      <c r="I36" s="3"/>
       <c r="J36" s="3">
-        <v>18.2</v>
-      </c>
-      <c r="K36" s="3">
-        <v>14.1</v>
-      </c>
-      <c r="L36" s="3"/>
+        <v>8.5</v>
+      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
-        <v>15</v>
-      </c>
-      <c r="J37" s="3">
-        <v>18.399999999999999</v>
-      </c>
+        <v>6.3</v>
+      </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3">
-        <v>16</v>
-      </c>
-      <c r="J38" s="3">
-        <v>18.5</v>
-      </c>
+        <v>6.4</v>
+      </c>
+      <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D39" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-      <c r="J39" s="3">
-        <v>19</v>
-      </c>
-      <c r="K39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3">
+        <v>16.2</v>
+      </c>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D40" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-      <c r="J40" s="3">
-        <v>19</v>
-      </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="J40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="K40" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D41" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
       <c r="J41" s="3">
-        <v>19</v>
-      </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K41" s="3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L41" s="3">
+        <v>14.4</v>
+      </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -1933,21 +2047,24 @@
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
       <c r="J42" s="3">
-        <v>19</v>
-      </c>
-      <c r="K42" s="3"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K42" s="3">
+        <v>18.3</v>
+      </c>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -1955,21 +2072,26 @@
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3">
-        <v>19</v>
-      </c>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K43" s="3">
+        <v>18.2</v>
+      </c>
+      <c r="L43" s="3">
+        <v>14.1</v>
+      </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1977,21 +2099,24 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3">
-        <v>19</v>
-      </c>
-      <c r="K44" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="K44" s="3">
+        <v>18.399999999999999</v>
+      </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1999,368 +2124,392 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3">
-        <v>19</v>
-      </c>
-      <c r="K45" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="K45" s="3">
+        <v>18.5</v>
+      </c>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="3">
-        <v>14.5</v>
-      </c>
-      <c r="J46" s="3">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="K46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3">
+        <v>19</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="3">
-        <v>20.2</v>
-      </c>
-      <c r="K47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3">
+        <v>19</v>
+      </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
-      <c r="J48" s="3">
-        <v>20.3</v>
-      </c>
-      <c r="K48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3">
+        <v>19</v>
+      </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="3"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
       <c r="I49" s="3"/>
-      <c r="J49" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="K49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3">
+        <v>19</v>
+      </c>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" s="3"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="K50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3">
+        <v>19</v>
+      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="3"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
-      <c r="J51" s="3">
-        <v>21.5</v>
-      </c>
-      <c r="K51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3">
+        <v>19</v>
+      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
-      <c r="J52" s="3">
-        <v>21.4</v>
-      </c>
-      <c r="K52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3">
+        <v>19</v>
+      </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
       <c r="J53" s="3">
-        <v>20.5</v>
-      </c>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="M53" s="3">
-        <v>6.8</v>
-      </c>
+        <v>14.5</v>
+      </c>
+      <c r="K53" s="3">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
       <c r="N53" s="3"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="D54" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="K54" s="3">
+        <v>20.2</v>
+      </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" s="3"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B55" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3">
-        <v>9</v>
-      </c>
+      <c r="K55" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="L55" s="3"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" s="3"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3">
-        <v>10</v>
-      </c>
+      <c r="K56" s="3">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" s="3"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B57" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3">
-        <v>10</v>
-      </c>
+      <c r="K57" s="3">
+        <v>20.5</v>
+      </c>
+      <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" s="3"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3" t="s">
-        <v>110</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
+      <c r="K58" s="3">
+        <v>21.5</v>
+      </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" s="3"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3" t="s">
-        <v>110</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E59" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
+      <c r="K59" s="3">
+        <v>21.4</v>
+      </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" s="3"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>111</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
+      <c r="K60" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M60" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="N60" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="O60" s="3"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B61" s="3"/>
-      <c r="C61" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -2371,18 +2520,15 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61" s="3"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -2391,20 +2537,19 @@
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
+      <c r="M62" s="3">
+        <v>9</v>
+      </c>
       <c r="N62" s="3"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62" s="3"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2413,20 +2558,19 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
+      <c r="M63" s="3">
+        <v>10</v>
+      </c>
       <c r="N63" s="3"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63" s="3"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B64" s="3"/>
-      <c r="C64" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -2435,19 +2579,22 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
+      <c r="M64" s="3">
+        <v>10</v>
+      </c>
       <c r="N64" s="3"/>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64" s="3"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -2459,15 +2606,182 @@
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="O71" s="3"/>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
+      <c r="M72" s="3"/>
+      <c r="N72" s="3"/>
+      <c r="O72" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N64" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N65">
-    <sortCondition ref="G2:G65"/>
+  <autoFilter ref="A1:O71" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O72">
+    <sortCondition ref="H2:H72"/>
   </sortState>
-  <conditionalFormatting sqref="A2:N13 A25:N64 A14:C24 E14:N19 E23:N24 F20:N22 D20:D22 A65">
+  <mergeCells count="3">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A14"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A2:O2 A32:O71 A21:C31 E21:O26 E30:O31 F27:O29 D27:D29 A72 A5:O8 B3:O4 A15:O20 B9:F10 A11:F12 B13:F14 G9:O14">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$G2="Completed"</formula>
+      <formula>$H2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
migrate: move all my other files to this repo.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE5DB18-BEE7-F14B-BD8E-4837EAFD50E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C3E053-9D5B-4C4C-9E79-8DAA9E8E4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$73</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="134">
   <si>
     <t>Topic</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>Consider linking logistic regression's implementation to here.</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
   </si>
 </sst>
 </file>
@@ -453,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +466,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -539,13 +548,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -872,16 +885,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
@@ -1125,7 +1138,9 @@
         <v>32</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1149,7 +1164,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>20</v>
@@ -1160,7 +1175,9 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
@@ -1170,7 +1187,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>20</v>
@@ -1181,21 +1198,23 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="2" t="s">
-        <v>128</v>
+      <c r="O10" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>121</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>20</v>
@@ -1206,26 +1225,22 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3" t="s">
-        <v>127</v>
-      </c>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1236,19 +1251,19 @@
       <c r="O12" s="3"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1259,7 +1274,9 @@
       <c r="O13" s="3"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
+      <c r="A14" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>130</v>
@@ -1268,10 +1285,10 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
@@ -1279,59 +1296,59 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="3" t="s">
-        <v>132</v>
-      </c>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="C15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3">
-        <v>8.1</v>
-      </c>
+      <c r="L15" s="3"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1343,12 +1360,10 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="3">
-        <v>17</v>
-      </c>
+      <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3">
-        <v>8.3000000000000007</v>
+        <v>8.1</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1356,7 +1371,7 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1371,7 +1386,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3">
-        <v>8.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1379,26 +1394,24 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="3">
-        <v>17.3</v>
-      </c>
+      <c r="J19" s="3">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3"/>
       <c r="L19" s="3">
-        <v>7.1</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -1406,12 +1419,12 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1419,11 +1432,9 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="3">
-        <v>17.2</v>
-      </c>
+      <c r="K20" s="3"/>
       <c r="L20" s="3">
-        <v>6.4</v>
+        <v>8.4</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -1431,7 +1442,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1443,12 +1454,14 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="K21" s="3">
-        <v>17</v>
+        <v>17.3</v>
       </c>
       <c r="L21" s="3">
-        <v>6</v>
+        <v>7.1</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -1456,30 +1469,24 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>45</v>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
+        <v>17.2</v>
       </c>
       <c r="L22" s="3">
-        <v>3.1</v>
+        <v>6.4</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1487,30 +1494,24 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-      <c r="J23" s="3">
-        <v>3.4</v>
-      </c>
+      <c r="J23" s="3"/>
       <c r="K23" s="3">
-        <v>11.3</v>
+        <v>17</v>
       </c>
       <c r="L23" s="3">
-        <v>3.1</v>
+        <v>6</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -1518,7 +1519,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>18</v>
@@ -1535,10 +1536,10 @@
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="K24" s="3">
-        <v>11.4</v>
+        <v>3.2</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="L24" s="3">
         <v>3.1</v>
@@ -1549,7 +1550,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>18</v>
@@ -1565,12 +1566,14 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="3">
+        <v>3.4</v>
+      </c>
       <c r="K25" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>49</v>
+        <v>11.3</v>
+      </c>
+      <c r="L25" s="3">
+        <v>3.1</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -1578,7 +1581,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>18</v>
@@ -1589,25 +1592,27 @@
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L26" s="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="K26" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="L26" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>18</v>
@@ -1618,25 +1623,25 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>18</v>
@@ -1644,9 +1649,7 @@
       <c r="C28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
         <v>19</v>
@@ -1655,21 +1658,19 @@
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3">
-        <v>4.5</v>
+        <v>4.3</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>18</v>
@@ -1677,9 +1678,7 @@
       <c r="C29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
         <v>19</v>
@@ -1688,21 +1687,19 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>18</v>
@@ -1720,10 +1717,14 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="J30" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="L30" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
@@ -1731,7 +1732,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>18</v>
@@ -1739,7 +1740,9 @@
       <c r="C31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
         <v>19</v>
@@ -1747,12 +1750,14 @@
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3">
-        <v>10.5</v>
+      <c r="J31" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
@@ -1760,7 +1765,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>18</v>
@@ -1768,47 +1773,49 @@
       <c r="C32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="3">
-        <v>12</v>
-      </c>
-      <c r="L32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3">
-        <v>13.3</v>
-      </c>
+      <c r="J33" s="3"/>
       <c r="K33" s="3">
-        <v>16.100000000000001</v>
+        <v>10.5</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
@@ -1816,22 +1823,24 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="K34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3">
+        <v>12</v>
+      </c>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -1839,26 +1848,30 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C35" s="3" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3">
-        <v>9.1999999999999993</v>
+      <c r="J35" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="K35" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -1866,219 +1879,217 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3">
-        <v>8.5</v>
+        <v>13.4</v>
       </c>
       <c r="K36" s="3"/>
-      <c r="L36" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="D37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3">
-        <v>6.3</v>
-      </c>
+      <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="L37" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
-      <c r="O37" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="O37" s="3"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3">
+        <v>8.5</v>
+      </c>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
+      <c r="L38" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
+      <c r="I39" s="3">
+        <v>6.3</v>
+      </c>
       <c r="J39" s="3"/>
-      <c r="K39" s="3">
-        <v>16.2</v>
-      </c>
+      <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K40" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="L40" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="I40" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="3">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="J41" s="3"/>
       <c r="K41" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L41" s="3">
-        <v>14.4</v>
-      </c>
+        <v>16.2</v>
+      </c>
+      <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
+      <c r="O41" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D42" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-      <c r="J42" s="3">
-        <v>8.6999999999999993</v>
+      <c r="J42" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="K42" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="L42" s="3"/>
+        <v>16.3</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D43" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
       <c r="J43" s="3">
-        <v>8.8000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="K43" s="3">
-        <v>18.2</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="L43" s="3">
-        <v>14.1</v>
+        <v>14.4</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2086,7 +2097,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2099,10 +2110,10 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3">
-        <v>15</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="K44" s="3">
-        <v>18.399999999999999</v>
+        <v>18.3</v>
       </c>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
@@ -2111,7 +2122,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2124,33 +2135,37 @@
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
       <c r="J45" s="3">
-        <v>16</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K45" s="3">
-        <v>18.5</v>
-      </c>
-      <c r="L45" s="3"/>
+        <v>18.2</v>
+      </c>
+      <c r="L45" s="3">
+        <v>14.1</v>
+      </c>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
       <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="3">
+        <v>15</v>
+      </c>
       <c r="K46" s="3">
-        <v>19</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
@@ -2159,21 +2174,23 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="3">
+        <v>16</v>
+      </c>
       <c r="K47" s="3">
-        <v>19</v>
+        <v>18.5</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -2182,7 +2199,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2205,7 +2222,7 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2228,7 +2245,7 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2251,7 +2268,7 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2274,7 +2291,7 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -2297,25 +2314,21 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="J53" s="3">
-        <v>14.5</v>
-      </c>
+      <c r="J53" s="3"/>
       <c r="K53" s="3">
-        <v>20.100000000000001</v>
+        <v>19</v>
       </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
@@ -2324,14 +2337,12 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -2340,7 +2351,7 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3">
-        <v>20.2</v>
+        <v>19</v>
       </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
@@ -2349,7 +2360,7 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>32</v>
@@ -2363,9 +2374,11 @@
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
+      <c r="J55" s="3">
+        <v>14.5</v>
+      </c>
       <c r="K55" s="3">
-        <v>20.3</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
@@ -2374,7 +2387,7 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>32</v>
@@ -2390,7 +2403,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3">
-        <v>20.399999999999999</v>
+        <v>20.2</v>
       </c>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
@@ -2399,7 +2412,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>32</v>
@@ -2415,7 +2428,7 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3">
-        <v>20.5</v>
+        <v>20.3</v>
       </c>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
@@ -2424,25 +2437,23 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3">
-        <v>21.5</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
@@ -2451,25 +2462,23 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3">
-        <v>21.4</v>
+        <v>20.5</v>
       </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
@@ -2478,45 +2487,53 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3">
-        <v>20.5</v>
+        <v>21.5</v>
       </c>
       <c r="L60" s="3"/>
-      <c r="M60" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="N60" s="3">
-        <v>6.8</v>
-      </c>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
       <c r="O60" s="3"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B61" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
+      <c r="K61" s="3">
+        <v>21.4</v>
+      </c>
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
@@ -2524,9 +2541,11 @@
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2535,17 +2554,21 @@
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
+      <c r="K62" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L62" s="3"/>
       <c r="M62" s="3">
-        <v>9</v>
-      </c>
-      <c r="N62" s="3"/>
+        <v>15.1</v>
+      </c>
+      <c r="N62" s="3">
+        <v>6.8</v>
+      </c>
       <c r="O62" s="3"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2558,15 +2581,13 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="3">
-        <v>10</v>
-      </c>
+      <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -2580,22 +2601,18 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B65" s="3"/>
-      <c r="C65" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2604,21 +2621,19 @@
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
+      <c r="M65" s="3">
+        <v>10</v>
+      </c>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B66" s="3"/>
-      <c r="C66" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -2627,13 +2642,15 @@
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
+      <c r="M66" s="3">
+        <v>10</v>
+      </c>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3" t="s">
@@ -2656,7 +2673,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3" t="s">
@@ -2679,14 +2696,14 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -2702,14 +2719,14 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -2725,7 +2742,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3" t="s">
@@ -2748,11 +2765,11 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>116</v>
@@ -2769,17 +2786,64 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
     </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+      <c r="M73" s="3"/>
+      <c r="N73" s="3"/>
+      <c r="O73" s="3"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O71" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O72">
-    <sortCondition ref="H2:H72"/>
+  <autoFilter ref="A1:O73" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O74">
+    <sortCondition ref="H2:H74"/>
   </sortState>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:O2 A32:O71 A21:C31 E21:O26 E30:O31 F27:O29 D27:D29 A72 A5:O8 B3:O4 A15:O20 B9:F10 A11:F12 B13:F14 G9:O14">
+  <conditionalFormatting sqref="A2:O2 A34:O73 A23:C33 E23:O28 E32:O33 F29:O31 D29:D31 A74 A5:O8 B3:O4 A17:O22 B9:F10 A11:F11 B15:F16 G8:G10 G9:O16 A14:F14 B12:F13">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$H2="Completed"</formula>
     </cfRule>

</xml_diff>

<commit_message>
migrate: move chapters 4-5 of probability theory to this repo.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22746915-78F6-764D-AC87-E9CBF85EB2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CBFB44-8A95-FA46-915D-5EB8510C5DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="150">
   <si>
     <t>Topic</t>
   </si>
@@ -368,42 +368,12 @@
     <t>GRU</t>
   </si>
   <si>
-    <t>Bernoulli</t>
-  </si>
-  <si>
-    <t>Univariate Distributions</t>
-  </si>
-  <si>
     <t>Discrete Random Variables</t>
   </si>
   <si>
-    <t>Binomial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poisson </t>
-  </si>
-  <si>
-    <t>Geometric</t>
-  </si>
-  <si>
-    <t>Uniform</t>
-  </si>
-  <si>
     <t>Continuous Random Variables</t>
   </si>
   <si>
-    <t>Exponential</t>
-  </si>
-  <si>
-    <t>Gaussian</t>
-  </si>
-  <si>
-    <t>Multivariate Gaussian</t>
-  </si>
-  <si>
-    <t>Multivariate Distributions</t>
-  </si>
-  <si>
     <t>Voronoi Region</t>
   </si>
   <si>
@@ -501,6 +471,24 @@
   </si>
   <si>
     <t>Geometric Distribution</t>
+  </si>
+  <si>
+    <t>IID</t>
+  </si>
+  <si>
+    <t>Probability Density Function</t>
+  </si>
+  <si>
+    <t>Mean, Median and Mode</t>
+  </si>
+  <si>
+    <t>Continuous Uniform Distribution</t>
+  </si>
+  <si>
+    <t>Exponential Distribution</t>
+  </si>
+  <si>
+    <t>Gaussian Distribution</t>
   </si>
 </sst>
 </file>
@@ -617,6 +605,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -626,7 +618,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -636,34 +627,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1107,8 +1075,8 @@
   <dimension ref="A1:O125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59:A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1147,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1175,7 +1143,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1194,7 +1162,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>20</v>
@@ -1214,14 +1182,14 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>20</v>
@@ -1235,14 +1203,14 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>20</v>
@@ -1341,7 +1309,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1358,7 +1326,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>20</v>
@@ -1376,7 +1344,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
@@ -1385,7 +1353,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>20</v>
@@ -1397,11 +1365,11 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>30</v>
@@ -1410,7 +1378,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>20</v>
@@ -1422,22 +1390,22 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>121</v>
+      <c r="A11" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>20</v>
@@ -1451,19 +1419,19 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1474,19 +1442,19 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -1497,18 +1465,18 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>129</v>
+      <c r="A14" s="8" t="s">
+        <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>20</v>
@@ -1522,16 +1490,16 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>20</v>
@@ -1545,19 +1513,19 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="4" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -1566,21 +1534,23 @@
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1594,16 +1564,18 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
+      <c r="G18" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1617,16 +1589,18 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="9"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H19" s="4" t="s">
         <v>20</v>
       </c>
@@ -1640,18 +1614,20 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="9"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
+      <c r="G20" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1665,18 +1641,20 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="9"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
+      <c r="G21" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H21" s="4" t="s">
         <v>20</v>
       </c>
@@ -1690,18 +1668,20 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
+      <c r="G22" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H22" s="4" t="s">
         <v>20</v>
       </c>
@@ -1715,18 +1695,20 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="9"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H23" s="4" t="s">
         <v>20</v>
       </c>
@@ -1740,18 +1722,20 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="9"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H24" s="4" t="s">
         <v>20</v>
       </c>
@@ -1765,18 +1749,20 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="9"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
+      <c r="G25" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H25" s="4" t="s">
         <v>20</v>
       </c>
@@ -1790,18 +1776,20 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="9"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H26" s="4" t="s">
         <v>20</v>
       </c>
@@ -1815,18 +1803,20 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="9"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H27" s="4" t="s">
         <v>20</v>
       </c>
@@ -1840,18 +1830,20 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="9"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H28" s="4" t="s">
         <v>20</v>
       </c>
@@ -1865,18 +1857,20 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="9"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H29" s="4" t="s">
         <v>20</v>
       </c>
@@ -1890,18 +1884,20 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="9"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="H30" s="4" t="s">
         <v>20</v>
       </c>
@@ -1914,22 +1910,22 @@
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
-        <v>148</v>
+      <c r="A31" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E31" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E31" s="7"/>
       <c r="F31" s="4"/>
       <c r="G31" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>20</v>
@@ -1943,23 +1939,23 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
+      <c r="A32" s="9"/>
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -1970,20 +1966,20 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E33" s="7"/>
       <c r="F33" s="4"/>
       <c r="G33" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>20</v>
@@ -1997,22 +1993,22 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>150</v>
+      <c r="A34" s="8" t="s">
+        <v>140</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E34" s="7"/>
       <c r="F34" s="4"/>
       <c r="G34" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>20</v>
@@ -2026,23 +2022,23 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+      <c r="A35" s="9"/>
       <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E35" s="7"/>
       <c r="F35" s="4"/>
       <c r="G35" s="5" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -2053,20 +2049,20 @@
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E36" s="7"/>
       <c r="F36" s="4"/>
       <c r="G36" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>20</v>
@@ -2080,20 +2076,22 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>151</v>
+      <c r="A37" s="8" t="s">
+        <v>141</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D37" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E37" s="7"/>
       <c r="F37" s="4"/>
       <c r="G37" s="5" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>20</v>
@@ -2107,20 +2105,24 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
-      <c r="B38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="3"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D38" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E38" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H38" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
@@ -2130,18 +2132,20 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="3"/>
+      <c r="C39" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="D39" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="9"/>
+        <v>139</v>
+      </c>
+      <c r="E39" s="7"/>
       <c r="F39" s="4"/>
       <c r="G39" s="5" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="H39" s="4" t="s">
         <v>20</v>
@@ -2155,16 +2159,26 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
+      <c r="A40" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="B40" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="9"/>
+      <c r="C40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="7"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="4"/>
+      <c r="G40" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2174,18 +2188,24 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="9"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="4"/>
+      <c r="G41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -2195,18 +2215,24 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="13" t="s">
-        <v>152</v>
-      </c>
+      <c r="A42" s="10"/>
       <c r="B42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="9"/>
+      <c r="C42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E42" s="7"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="4"/>
+      <c r="G42" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -2216,18 +2242,26 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="13" t="s">
-        <v>153</v>
+      <c r="A43" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="9"/>
+      <c r="C43" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" s="7"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="4"/>
+      <c r="G43" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2237,16 +2271,24 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="9"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="4"/>
+      <c r="G44" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -2256,16 +2298,24 @@
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="9"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="4"/>
+      <c r="G45" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -2275,16 +2325,20 @@
       <c r="O45" s="4"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
+      <c r="A46" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="B46" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="9"/>
+      <c r="E46" s="7"/>
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
-      <c r="H46" s="4"/>
+      <c r="H46" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
@@ -2294,13 +2348,19 @@
       <c r="O46" s="4"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
+      <c r="A47" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="9"/>
+      <c r="C47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47" s="7"/>
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
       <c r="H47" s="4"/>
@@ -2313,13 +2373,15 @@
       <c r="O47" s="4"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
+      <c r="A48" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="B48" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="9"/>
+      <c r="E48" s="7"/>
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
       <c r="H48" s="4"/>
@@ -2332,13 +2394,15 @@
       <c r="O48" s="4"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
+      <c r="A49" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="B49" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="9"/>
+      <c r="E49" s="7"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
       <c r="H49" s="4"/>
@@ -2351,13 +2415,15 @@
       <c r="O49" s="4"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
+      <c r="A50" s="6" t="s">
+        <v>136</v>
+      </c>
       <c r="B50" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="9"/>
+      <c r="E50" s="7"/>
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
       <c r="H50" s="4"/>
@@ -2370,13 +2436,15 @@
       <c r="O50" s="4"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+      <c r="A51" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="B51" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="9"/>
+      <c r="E51" s="7"/>
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
       <c r="H51" s="4"/>
@@ -2389,13 +2457,15 @@
       <c r="O51" s="4"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+      <c r="A52" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="B52" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="7"/>
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
       <c r="H52" s="4"/>
@@ -2408,13 +2478,15 @@
       <c r="O52" s="4"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="2"/>
+      <c r="A53" s="11" t="s">
+        <v>147</v>
+      </c>
       <c r="B53" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="9"/>
+      <c r="E53" s="7"/>
       <c r="F53" s="4"/>
       <c r="G53" s="5"/>
       <c r="H53" s="4"/>
@@ -2427,13 +2499,13 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="2"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="9"/>
+      <c r="E54" s="7"/>
       <c r="F54" s="4"/>
       <c r="G54" s="5"/>
       <c r="H54" s="4"/>
@@ -2446,13 +2518,13 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="2"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="9"/>
+      <c r="E55" s="7"/>
       <c r="F55" s="4"/>
       <c r="G55" s="5"/>
       <c r="H55" s="4"/>
@@ -2465,13 +2537,15 @@
       <c r="O55" s="4"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="2"/>
+      <c r="A56" s="11" t="s">
+        <v>148</v>
+      </c>
       <c r="B56" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="9"/>
+      <c r="E56" s="7"/>
       <c r="F56" s="4"/>
       <c r="G56" s="5"/>
       <c r="H56" s="4"/>
@@ -2484,13 +2558,13 @@
       <c r="O56" s="4"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="9"/>
+      <c r="E57" s="7"/>
       <c r="F57" s="4"/>
       <c r="G57" s="5"/>
       <c r="H57" s="4"/>
@@ -2503,13 +2577,13 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="9"/>
+      <c r="E58" s="7"/>
       <c r="F58" s="4"/>
       <c r="G58" s="5"/>
       <c r="H58" s="4"/>
@@ -2522,13 +2596,15 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="2"/>
+      <c r="A59" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="B59" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="9"/>
+      <c r="E59" s="7"/>
       <c r="F59" s="4"/>
       <c r="G59" s="5"/>
       <c r="H59" s="4"/>
@@ -2541,13 +2617,13 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="2"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="9"/>
+      <c r="E60" s="7"/>
       <c r="F60" s="4"/>
       <c r="G60" s="5"/>
       <c r="H60" s="4"/>
@@ -2560,13 +2636,13 @@
       <c r="O60" s="4"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="2"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="9"/>
+      <c r="E61" s="7"/>
       <c r="F61" s="4"/>
       <c r="G61" s="5"/>
       <c r="H61" s="4"/>
@@ -2585,7 +2661,7 @@
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="9"/>
+      <c r="E62" s="7"/>
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
       <c r="H62" s="4"/>
@@ -2604,7 +2680,7 @@
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="9"/>
+      <c r="E63" s="7"/>
       <c r="F63" s="4"/>
       <c r="G63" s="5"/>
       <c r="H63" s="4"/>
@@ -2623,7 +2699,7 @@
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="9"/>
+      <c r="E64" s="7"/>
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
       <c r="H64" s="4"/>
@@ -2642,7 +2718,7 @@
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
-      <c r="E65" s="9"/>
+      <c r="E65" s="7"/>
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
       <c r="H65" s="4"/>
@@ -2661,7 +2737,7 @@
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
-      <c r="E66" s="9"/>
+      <c r="E66" s="7"/>
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
       <c r="H66" s="4"/>
@@ -2680,7 +2756,7 @@
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="9"/>
+      <c r="E67" s="7"/>
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
       <c r="H67" s="4"/>
@@ -3252,7 +3328,7 @@
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>31</v>
@@ -3995,16 +4071,10 @@
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A118" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="A118" s="3"/>
       <c r="B118" s="3"/>
-      <c r="C118" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
@@ -4018,16 +4088,10 @@
       <c r="O118" s="3"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
-        <v>112</v>
-      </c>
+      <c r="A119" s="3"/>
       <c r="B119" s="3"/>
-      <c r="C119" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
@@ -4041,16 +4105,10 @@
       <c r="O119" s="3"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A120" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="A120" s="3"/>
       <c r="B120" s="3"/>
-      <c r="C120" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
@@ -4064,16 +4122,10 @@
       <c r="O120" s="3"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="A121" s="3"/>
       <c r="B121" s="3"/>
-      <c r="C121" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D121" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
@@ -4087,16 +4139,10 @@
       <c r="O121" s="3"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="A122" s="3"/>
       <c r="B122" s="3"/>
-      <c r="C122" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
@@ -4110,16 +4156,10 @@
       <c r="O122" s="3"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
-        <v>117</v>
-      </c>
+      <c r="A123" s="3"/>
       <c r="B123" s="3"/>
-      <c r="C123" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
@@ -4133,16 +4173,10 @@
       <c r="O123" s="3"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="A124" s="3"/>
       <c r="B124" s="3"/>
-      <c r="C124" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D124" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -4156,16 +4190,10 @@
       <c r="O124" s="3"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="A125" s="3"/>
       <c r="B125" s="3"/>
-      <c r="C125" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
@@ -4183,7 +4211,12 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O125">
     <sortCondition ref="H2:H125"/>
   </sortState>
-  <mergeCells count="7">
+  <mergeCells count="12">
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A2:A4"/>
@@ -4192,63 +4225,63 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A31:A33"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:O2 A85:O124 A74:C84 E74:O79 E83:O84 F80:O82 D80:D82 A125 A5:O8 B3:O4 A68:O73 G8:G10 B9:F10 A11 A14 D11:F67 B11:B67 G9:O67">
-    <cfRule type="expression" dxfId="14" priority="13">
+  <conditionalFormatting sqref="A2:O2 A85:O124 A74:C84 E74:O79 E83:O84 F80:O82 D80:D82 A125 A5:O8 B3:O4 A68:O73 G8:G10 B9:F10 A11 A14 B11:B67 D11:F67 G9:O67">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$H2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A31 A51:A67">
-    <cfRule type="expression" dxfId="13" priority="12">
+  <conditionalFormatting sqref="A17:A31 A51:A53 A56 A59 A62:A67">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$H17="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C24">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$H20="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$H11="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$H14="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C19">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$H17="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C13">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$H12="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$H16="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$H25="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26:C30">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$H26="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C36">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="C33:C43">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$H33="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$H31="Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
migrate: migrate the remaining to this repo.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CBFB44-8A95-FA46-915D-5EB8510C5DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DA097-CE13-6C4F-BEFA-1306C341E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$124</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$135</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="161">
   <si>
     <t>Topic</t>
   </si>
@@ -489,16 +489,56 @@
   </si>
   <si>
     <t>Gaussian Distribution</t>
+  </si>
+  <si>
+    <t>Joint Distributions</t>
+  </si>
+  <si>
+    <t>Multivariate</t>
+  </si>
+  <si>
+    <t>Joint PMF and PDF</t>
+  </si>
+  <si>
+    <t>Joint Expectation and Correlation</t>
+  </si>
+  <si>
+    <t>Conditional PMF and PDF</t>
+  </si>
+  <si>
+    <t>Conditional Expectation and Variance</t>
+  </si>
+  <si>
+    <t>Sum of Random Variables</t>
+  </si>
+  <si>
+    <t>Random Vectors</t>
+  </si>
+  <si>
+    <t>Multivariate Gaussian Distribution</t>
+  </si>
+  <si>
+    <t>Moment Generating and Characteristic Functions</t>
+  </si>
+  <si>
+    <t>Probability Inequalities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -594,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -618,14 +658,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1072,16 +1107,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:O125"/>
+  <dimension ref="A1:O136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59:A61"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
@@ -2363,7 +2398,9 @@
       <c r="E47" s="7"/>
       <c r="F47" s="4"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
@@ -2379,12 +2416,18 @@
       <c r="B48" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
+      <c r="C48" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E48" s="7"/>
       <c r="F48" s="4"/>
       <c r="G48" s="5"/>
-      <c r="H48" s="4"/>
+      <c r="H48" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -2400,12 +2443,18 @@
       <c r="B49" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="4"/>
+      <c r="C49" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E49" s="7"/>
       <c r="F49" s="4"/>
       <c r="G49" s="5"/>
-      <c r="H49" s="4"/>
+      <c r="H49" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
@@ -2421,12 +2470,18 @@
       <c r="B50" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
+      <c r="C50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E50" s="7"/>
       <c r="F50" s="4"/>
       <c r="G50" s="5"/>
-      <c r="H50" s="4"/>
+      <c r="H50" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -2442,12 +2497,18 @@
       <c r="B51" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="4"/>
+      <c r="C51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E51" s="7"/>
       <c r="F51" s="4"/>
       <c r="G51" s="5"/>
-      <c r="H51" s="4"/>
+      <c r="H51" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -2457,18 +2518,24 @@
       <c r="O51" s="4"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="7"/>
+      <c r="B52" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="5"/>
-      <c r="H52" s="4"/>
+      <c r="H52" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -2478,18 +2545,26 @@
       <c r="O52" s="4"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="8" t="s">
         <v>147</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="4"/>
+      <c r="C53" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E53" s="7"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="4"/>
+      <c r="G53" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
@@ -2499,16 +2574,24 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="12"/>
+      <c r="A54" s="9"/>
       <c r="B54" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="4"/>
+      <c r="C54" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E54" s="7"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="4"/>
+      <c r="G54" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -2518,16 +2601,24 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="4"/>
+      <c r="C55" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E55" s="7"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="4"/>
+      <c r="G55" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -2537,18 +2628,26 @@
       <c r="O55" s="4"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="8" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="4"/>
+      <c r="C56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E56" s="7"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="4"/>
+      <c r="G56" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
@@ -2558,16 +2657,24 @@
       <c r="O56" s="4"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="12"/>
-      <c r="B57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="7"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="4"/>
+      <c r="G57" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -2577,16 +2684,24 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
-      <c r="B58" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="7"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="4"/>
+      <c r="G58" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -2596,18 +2711,26 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="8" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="4"/>
+      <c r="C59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E59" s="7"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="4"/>
+      <c r="G59" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -2617,16 +2740,24 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="12"/>
-      <c r="B60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="7"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="4"/>
+      <c r="G60" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -2636,16 +2767,24 @@
       <c r="O60" s="4"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
-      <c r="B61" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="7"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="4"/>
+      <c r="G61" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -2655,12 +2794,18 @@
       <c r="O61" s="4"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="2"/>
+      <c r="A62" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="B62" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="4"/>
+      <c r="C62" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E62" s="7"/>
       <c r="F62" s="4"/>
       <c r="G62" s="5"/>
@@ -2674,12 +2819,18 @@
       <c r="O62" s="4"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
+      <c r="A63" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="B63" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="4"/>
+      <c r="C63" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E63" s="7"/>
       <c r="F63" s="4"/>
       <c r="G63" s="5"/>
@@ -2693,12 +2844,18 @@
       <c r="O63" s="4"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="2"/>
+      <c r="A64" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="B64" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="4"/>
+      <c r="C64" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E64" s="7"/>
       <c r="F64" s="4"/>
       <c r="G64" s="5"/>
@@ -2712,12 +2869,18 @@
       <c r="O64" s="4"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="2"/>
+      <c r="A65" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="B65" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="4"/>
+      <c r="C65" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E65" s="7"/>
       <c r="F65" s="4"/>
       <c r="G65" s="5"/>
@@ -2731,12 +2894,18 @@
       <c r="O65" s="4"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="B66" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="4"/>
+      <c r="C66" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E66" s="7"/>
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
@@ -2750,12 +2919,18 @@
       <c r="O66" s="4"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="2"/>
+      <c r="A67" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="B67" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="4"/>
+      <c r="C67" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E67" s="7"/>
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
@@ -2769,384 +2944,322 @@
       <c r="O67" s="4"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3"/>
-      <c r="L68" s="3">
-        <v>8.1</v>
-      </c>
-      <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3"/>
+      <c r="A68" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
-      <c r="O69" s="3"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
-      <c r="J70" s="3">
-        <v>17</v>
-      </c>
-      <c r="K70" s="3"/>
-      <c r="L70" s="3">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="M70" s="3"/>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E70" s="7"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3">
-        <v>8.4</v>
-      </c>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
-      <c r="O71" s="3"/>
+      <c r="A71" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3"/>
-      <c r="J72" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K72" s="3">
-        <v>17.3</v>
-      </c>
-      <c r="L72" s="3">
-        <v>7.1</v>
-      </c>
-      <c r="M72" s="3"/>
-      <c r="N72" s="3"/>
-      <c r="O72" s="3"/>
+      <c r="A72" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="A73" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
+      <c r="I73" s="3">
+        <v>6.3</v>
+      </c>
       <c r="J73" s="3"/>
-      <c r="K73" s="3">
-        <v>17.2</v>
-      </c>
-      <c r="L73" s="3">
-        <v>6.4</v>
-      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
-      <c r="O73" s="3"/>
+      <c r="O73" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" s="3"/>
+      <c r="A74" s="6"/>
+      <c r="B74" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3">
-        <v>17</v>
-      </c>
-      <c r="L74" s="3">
-        <v>6</v>
-      </c>
-      <c r="M74" s="3"/>
-      <c r="N74" s="3"/>
-      <c r="O74" s="3"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A75" s="6"/>
       <c r="B75" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G75" s="3"/>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
-      <c r="J75" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="K75" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L75" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M75" s="3"/>
-      <c r="N75" s="3"/>
-      <c r="O75" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="A76" s="6"/>
       <c r="B76" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="K76" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="L76" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M76" s="3"/>
-      <c r="N76" s="3"/>
-      <c r="O76" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="A77" s="2"/>
       <c r="B77" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="K77" s="3">
-        <v>11.4</v>
-      </c>
-      <c r="L77" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M77" s="3"/>
-      <c r="N77" s="3"/>
-      <c r="O77" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="A78" s="2"/>
       <c r="B78" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="L78" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="C78" s="3"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D79" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E79" s="3"/>
-      <c r="F79" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K79" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3">
+        <v>8.1</v>
+      </c>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D80" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E80" s="3"/>
-      <c r="F80" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
-      <c r="J80" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E81" s="3"/>
-      <c r="F81" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
       <c r="J81" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3">
+        <v>8.3000000000000007</v>
       </c>
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
@@ -3154,32 +3267,22 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E82" s="3"/>
-      <c r="F82" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>59</v>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3">
+        <v>8.4</v>
       </c>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
@@ -3187,28 +3290,26 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E83" s="3"/>
-      <c r="F83" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-      <c r="L83" s="3" t="s">
-        <v>61</v>
+      <c r="J83" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K83" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L83" s="3">
+        <v>7.1</v>
       </c>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
@@ -3216,28 +3317,24 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D84" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E84" s="3"/>
-      <c r="F84" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="L84" s="3" t="s">
-        <v>63</v>
+        <v>17.2</v>
+      </c>
+      <c r="L84" s="3">
+        <v>6.4</v>
       </c>
       <c r="M84" s="3"/>
       <c r="N84" s="3"/>
@@ -3245,15 +3342,13 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D85" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -3261,39 +3356,41 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3">
-        <v>12</v>
-      </c>
-      <c r="L85" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="L85" s="3">
+        <v>6</v>
+      </c>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D86" s="3"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
+      <c r="F86" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="3">
-        <v>13.3</v>
-      </c>
-      <c r="K86" s="3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="L86" s="3" t="s">
-        <v>68</v>
+        <v>3.2</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L86" s="3">
+        <v>3.1</v>
       </c>
       <c r="M86" s="3"/>
       <c r="N86" s="3"/>
@@ -3301,49 +3398,61 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
+      <c r="F87" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="K87" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="L87" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M87" s="3"/>
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C88" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F88" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
+      <c r="J88" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="K88" s="3">
+        <v>11.4</v>
+      </c>
       <c r="L88" s="3">
-        <v>9.1999999999999993</v>
+        <v>3.1</v>
       </c>
       <c r="M88" s="3"/>
       <c r="N88" s="3"/>
@@ -3351,26 +3460,28 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F89" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-      <c r="J89" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="K89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3">
+        <v>11.7</v>
+      </c>
       <c r="L89" s="3" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
@@ -3378,51 +3489,57 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" s="3"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
-      <c r="I90" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L90" s="3"/>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
-      <c r="O90" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="O90" s="3"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
+      <c r="F91" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
-      <c r="I91" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="J91" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="L91" s="3"/>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
@@ -3430,57 +3547,65 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B92" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C92" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
+      <c r="F92" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="L92" s="3"/>
+      <c r="J92" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="M92" s="3"/>
       <c r="N92" s="3"/>
-      <c r="O92" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="O92" s="3"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
+      <c r="F93" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K93" s="3">
-        <v>16.3</v>
+      <c r="J93" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -3488,30 +3613,28 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B94" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C94" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="J94" s="3">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="K94" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L94" s="3">
-        <v>14.4</v>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="M94" s="3"/>
       <c r="N94" s="3"/>
@@ -3519,64 +3642,70 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
+      <c r="F95" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="3">
-        <v>8.6999999999999993</v>
-      </c>
+      <c r="J95" s="3"/>
       <c r="K95" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="L95" s="3"/>
+        <v>10.5</v>
+      </c>
+      <c r="L95" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="M95" s="3"/>
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="3">
-        <v>8.8000000000000007</v>
-      </c>
+      <c r="J96" s="3"/>
       <c r="K96" s="3">
-        <v>18.2</v>
-      </c>
-      <c r="L96" s="3">
-        <v>14.1</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="L96" s="3"/>
       <c r="M96" s="3"/>
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D97" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
@@ -3584,24 +3713,26 @@
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3">
-        <v>15</v>
+        <v>13.3</v>
       </c>
       <c r="K97" s="3">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="L97" s="3"/>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L97" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="M97" s="3"/>
       <c r="N97" s="3"/>
       <c r="O97" s="3"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -3609,11 +3740,9 @@
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3">
-        <v>16</v>
-      </c>
-      <c r="K98" s="3">
-        <v>18.5</v>
-      </c>
+        <v>13.4</v>
+      </c>
+      <c r="K98" s="3"/>
       <c r="L98" s="3"/>
       <c r="M98" s="3"/>
       <c r="N98" s="3"/>
@@ -3621,91 +3750,78 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
+      <c r="C99" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D99" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E99" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
-      <c r="K99" s="3">
-        <v>19</v>
-      </c>
-      <c r="L99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="M99" s="3"/>
       <c r="N99" s="3"/>
       <c r="O99" s="3"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E100" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3">
-        <v>19</v>
-      </c>
-      <c r="L100" s="3"/>
+      <c r="J100" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="M100" s="3"/>
       <c r="N100" s="3"/>
       <c r="O100" s="3"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3">
-        <v>19</v>
-      </c>
-      <c r="L101" s="3"/>
-      <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-    </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B102" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
+      <c r="I102" s="3">
+        <v>6.4</v>
+      </c>
       <c r="J102" s="3"/>
-      <c r="K102" s="3">
-        <v>19</v>
-      </c>
+      <c r="K102" s="3"/>
       <c r="L102" s="3"/>
       <c r="M102" s="3"/>
       <c r="N102" s="3"/>
@@ -3713,12 +3829,14 @@
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
+      <c r="C103" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D103" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
@@ -3727,69 +3845,85 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3">
-        <v>19</v>
+        <v>16.2</v>
       </c>
       <c r="L103" s="3"/>
       <c r="M103" s="3"/>
       <c r="N103" s="3"/>
-      <c r="O103" s="3"/>
+      <c r="O103" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D104" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
+      <c r="J104" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="K104" s="3">
-        <v>19</v>
-      </c>
-      <c r="L104" s="3"/>
+        <v>16.3</v>
+      </c>
+      <c r="L104" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M104" s="3"/>
       <c r="N104" s="3"/>
       <c r="O104" s="3"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
+      <c r="C105" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D105" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
+      <c r="F105" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
+      <c r="J105" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K105" s="3">
-        <v>19</v>
-      </c>
-      <c r="L105" s="3"/>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L105" s="3">
+        <v>14.4</v>
+      </c>
       <c r="M105" s="3"/>
       <c r="N105" s="3"/>
       <c r="O105" s="3"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
@@ -3797,10 +3931,10 @@
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="3">
-        <v>14.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="K106" s="3">
-        <v>20.100000000000001</v>
+        <v>18.3</v>
       </c>
       <c r="L106" s="3"/>
       <c r="M106" s="3"/>
@@ -3809,48 +3943,50 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
+      <c r="J107" s="3">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="K107" s="3">
-        <v>20.2</v>
-      </c>
-      <c r="L107" s="3"/>
+        <v>18.2</v>
+      </c>
+      <c r="L107" s="3">
+        <v>14.1</v>
+      </c>
       <c r="M107" s="3"/>
       <c r="N107" s="3"/>
       <c r="O107" s="3"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
-      <c r="J108" s="3"/>
+      <c r="J108" s="3">
+        <v>15</v>
+      </c>
       <c r="K108" s="3">
-        <v>20.3</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="L108" s="3"/>
       <c r="M108" s="3"/>
@@ -3859,23 +3995,23 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
+      <c r="J109" s="3">
+        <v>16</v>
+      </c>
       <c r="K109" s="3">
-        <v>20.399999999999999</v>
+        <v>18.5</v>
       </c>
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
@@ -3884,14 +4020,12 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B110" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
@@ -3900,7 +4034,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="L110" s="3"/>
       <c r="M110" s="3"/>
@@ -3909,25 +4043,21 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3">
-        <v>21.5</v>
+        <v>19</v>
       </c>
       <c r="L111" s="3"/>
       <c r="M111" s="3"/>
@@ -3936,25 +4066,21 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3">
-        <v>21.4</v>
+        <v>19</v>
       </c>
       <c r="L112" s="3"/>
       <c r="M112" s="3"/>
@@ -3963,13 +4089,13 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B113" s="3"/>
       <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -3977,31 +4103,31 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="L113" s="3"/>
-      <c r="M113" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="N113" s="3">
-        <v>6.8</v>
-      </c>
+      <c r="M113" s="3"/>
+      <c r="N113" s="3"/>
       <c r="O113" s="3"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="D114" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
+      <c r="K114" s="3">
+        <v>19</v>
+      </c>
       <c r="L114" s="3"/>
       <c r="M114" s="3"/>
       <c r="N114" s="3"/>
@@ -4009,172 +4135,238 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
+      <c r="D115" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
-      <c r="K115" s="3"/>
+      <c r="K115" s="3">
+        <v>19</v>
+      </c>
       <c r="L115" s="3"/>
-      <c r="M115" s="3">
-        <v>9</v>
-      </c>
+      <c r="M115" s="3"/>
       <c r="N115" s="3"/>
       <c r="O115" s="3"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
-      <c r="K116" s="3"/>
+      <c r="K116" s="3">
+        <v>19</v>
+      </c>
       <c r="L116" s="3"/>
-      <c r="M116" s="3">
-        <v>10</v>
-      </c>
+      <c r="M116" s="3"/>
       <c r="N116" s="3"/>
       <c r="O116" s="3"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B117" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
+      <c r="D117" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
-      <c r="J117" s="3"/>
-      <c r="K117" s="3"/>
+      <c r="J117" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="K117" s="3">
+        <v>20.100000000000001</v>
+      </c>
       <c r="L117" s="3"/>
-      <c r="M117" s="3">
-        <v>10</v>
-      </c>
+      <c r="M117" s="3"/>
       <c r="N117" s="3"/>
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
+      <c r="A118" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
-      <c r="K118" s="3"/>
+      <c r="K118" s="3">
+        <v>20.2</v>
+      </c>
       <c r="L118" s="3"/>
       <c r="M118" s="3"/>
       <c r="N118" s="3"/>
       <c r="O118" s="3"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
+      <c r="A119" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
-      <c r="K119" s="3"/>
+      <c r="K119" s="3">
+        <v>20.3</v>
+      </c>
       <c r="L119" s="3"/>
       <c r="M119" s="3"/>
       <c r="N119" s="3"/>
       <c r="O119" s="3"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
+      <c r="A120" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
+      <c r="D120" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
-      <c r="K120" s="3"/>
+      <c r="K120" s="3">
+        <v>20.399999999999999</v>
+      </c>
       <c r="L120" s="3"/>
       <c r="M120" s="3"/>
       <c r="N120" s="3"/>
       <c r="O120" s="3"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
+      <c r="A121" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
-      <c r="K121" s="3"/>
+      <c r="K121" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L121" s="3"/>
       <c r="M121" s="3"/>
       <c r="N121" s="3"/>
       <c r="O121" s="3"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
+      <c r="A122" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
+      <c r="D122" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
-      <c r="K122" s="3"/>
+      <c r="K122" s="3">
+        <v>21.5</v>
+      </c>
       <c r="L122" s="3"/>
       <c r="M122" s="3"/>
       <c r="N122" s="3"/>
       <c r="O122" s="3"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
+      <c r="A123" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
+      <c r="D123" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
-      <c r="K123" s="3"/>
+      <c r="K123" s="3">
+        <v>21.4</v>
+      </c>
       <c r="L123" s="3"/>
       <c r="M123" s="3"/>
       <c r="N123" s="3"/>
       <c r="O123" s="3"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
+      <c r="A124" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
@@ -4183,14 +4375,22 @@
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
+      <c r="K124" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
+      <c r="M124" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="N124" s="3">
+        <v>6.8</v>
+      </c>
       <c r="O124" s="3"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A125" s="3"/>
+      <c r="A125" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
@@ -4206,12 +4406,212 @@
       <c r="N125" s="3"/>
       <c r="O125" s="3"/>
     </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="3"/>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="3">
+        <v>9</v>
+      </c>
+      <c r="N126" s="3"/>
+      <c r="O126" s="3"/>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="3"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="3"/>
+      <c r="I127" s="3"/>
+      <c r="J127" s="3"/>
+      <c r="K127" s="3"/>
+      <c r="L127" s="3"/>
+      <c r="M127" s="3">
+        <v>10</v>
+      </c>
+      <c r="N127" s="3"/>
+      <c r="O127" s="3"/>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="3">
+        <v>10</v>
+      </c>
+      <c r="N128" s="3"/>
+      <c r="O128" s="3"/>
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+      <c r="E129" s="3"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="3"/>
+      <c r="I129" s="3"/>
+      <c r="J129" s="3"/>
+      <c r="K129" s="3"/>
+      <c r="L129" s="3"/>
+      <c r="M129" s="3"/>
+      <c r="N129" s="3"/>
+      <c r="O129" s="3"/>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+      <c r="E130" s="3"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="3"/>
+      <c r="I130" s="3"/>
+      <c r="J130" s="3"/>
+      <c r="K130" s="3"/>
+      <c r="L130" s="3"/>
+      <c r="M130" s="3"/>
+      <c r="N130" s="3"/>
+      <c r="O130" s="3"/>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="3"/>
+      <c r="M131" s="3"/>
+      <c r="N131" s="3"/>
+      <c r="O131" s="3"/>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="3"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="3"/>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A133" s="3"/>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="3"/>
+      <c r="I133" s="3"/>
+      <c r="J133" s="3"/>
+      <c r="K133" s="3"/>
+      <c r="L133" s="3"/>
+      <c r="M133" s="3"/>
+      <c r="N133" s="3"/>
+      <c r="O133" s="3"/>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="3"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="3"/>
+      <c r="I134" s="3"/>
+      <c r="J134" s="3"/>
+      <c r="K134" s="3"/>
+      <c r="L134" s="3"/>
+      <c r="M134" s="3"/>
+      <c r="N134" s="3"/>
+      <c r="O134" s="3"/>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="3"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="3"/>
+      <c r="I135" s="3"/>
+      <c r="J135" s="3"/>
+      <c r="K135" s="3"/>
+      <c r="L135" s="3"/>
+      <c r="M135" s="3"/>
+      <c r="N135" s="3"/>
+      <c r="O135" s="3"/>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="3"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="3"/>
+      <c r="I136" s="3"/>
+      <c r="J136" s="3"/>
+      <c r="K136" s="3"/>
+      <c r="L136" s="3"/>
+      <c r="M136" s="3"/>
+      <c r="N136" s="3"/>
+      <c r="O136" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O124" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O125">
-    <sortCondition ref="H2:H125"/>
+  <autoFilter ref="A1:O135" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O136">
+    <sortCondition ref="H2:H136"/>
   </sortState>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="A68:A70"/>
     <mergeCell ref="A40:A42"/>
     <mergeCell ref="A43:A45"/>
     <mergeCell ref="A53:A55"/>
@@ -4225,12 +4625,12 @@
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A31:A33"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:O2 A85:O124 A74:C84 E74:O79 E83:O84 F80:O82 D80:D82 A125 A5:O8 B3:O4 A68:O73 G8:G10 B9:F10 A11 A14 B11:B67 D11:F67 G9:O67">
+  <conditionalFormatting sqref="A2:O2 A85:C95 E85:O90 E94:O95 F91:O93 D91:D93 A136 A5:O8 B3:O4 A79:O84 G8:G10 B9:F10 A11 A14 A96:O100 A102:O135 G9:O72 D11:F72 D74:O78 B11:B72 B74:B78 A73:O73">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>$H2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A31 A51:A53 A56 A59 A62:A67">
+  <conditionalFormatting sqref="A17:A31 A51:A53 A56 A59 A62:A68 A77:A78">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>$H17="Completed"</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: update content on TF-IDF.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3DA097-CE13-6C4F-BEFA-1306C341E4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD35A8B-D160-D645-BA2F-F330C3E46D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$145</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="164">
   <si>
     <t>Topic</t>
   </si>
@@ -522,6 +522,15 @@
   </si>
   <si>
     <t>Probability Inequalities</t>
+  </si>
+  <si>
+    <t>TF-IDF</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>Vector Semantics and Embeddings</t>
   </si>
 </sst>
 </file>
@@ -634,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -649,6 +658,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -658,9 +671,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1107,11 +1128,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:O136"/>
+  <dimension ref="A1:O146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84:H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1199,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1217,7 +1238,7 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1238,7 +1259,7 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1344,7 +1365,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1379,7 +1400,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
@@ -1404,7 +1425,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>30</v>
@@ -1429,7 +1450,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1454,7 +1475,7 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="4" t="s">
         <v>123</v>
       </c>
@@ -1477,7 +1498,7 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
         <v>123</v>
       </c>
@@ -1500,7 +1521,7 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1525,7 +1546,7 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>120</v>
       </c>
@@ -1548,7 +1569,7 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
         <v>120</v>
       </c>
@@ -1945,7 +1966,7 @@
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="10" t="s">
         <v>138</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1974,7 +1995,7 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
@@ -2001,7 +2022,7 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="10"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
@@ -2028,7 +2049,7 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2057,7 +2078,7 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
@@ -2084,7 +2105,7 @@
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="10"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
@@ -2111,7 +2132,7 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="10" t="s">
         <v>141</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2140,7 +2161,7 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
@@ -2167,7 +2188,7 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
@@ -2194,7 +2215,7 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="10" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2223,7 +2244,7 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="4" t="s">
         <v>22</v>
       </c>
@@ -2250,7 +2271,7 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="3" t="s">
         <v>22</v>
       </c>
@@ -2277,7 +2298,7 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="10" t="s">
         <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2306,7 +2327,7 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="9"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
@@ -2333,7 +2354,7 @@
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="4" t="s">
         <v>22</v>
       </c>
@@ -2545,7 +2566,7 @@
       <c r="O52" s="4"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="10" t="s">
         <v>147</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2574,7 +2595,7 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="9"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="3" t="s">
         <v>22</v>
       </c>
@@ -2601,7 +2622,7 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="10"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="3" t="s">
         <v>22</v>
       </c>
@@ -2628,7 +2649,7 @@
       <c r="O55" s="4"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+      <c r="A56" s="10" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2657,7 +2678,7 @@
       <c r="O56" s="4"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="9"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="4" t="s">
         <v>22</v>
       </c>
@@ -2684,7 +2705,7 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
+      <c r="A58" s="12"/>
       <c r="B58" s="4" t="s">
         <v>22</v>
       </c>
@@ -2711,7 +2732,7 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="10" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -2740,7 +2761,7 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="9"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="4" t="s">
         <v>22</v>
       </c>
@@ -2767,7 +2788,7 @@
       <c r="O60" s="4"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="10"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="4" t="s">
         <v>22</v>
       </c>
@@ -2944,7 +2965,7 @@
       <c r="O67" s="4"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="10" t="s">
         <v>158</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -2973,7 +2994,7 @@
       <c r="O68" s="4"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="9"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="4" t="s">
         <v>22</v>
       </c>
@@ -3000,7 +3021,7 @@
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="3" t="s">
         <v>22</v>
       </c>
@@ -3056,7 +3077,7 @@
       <c r="B72" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D72" s="4"/>
@@ -3073,7 +3094,7 @@
       <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -3100,109 +3121,95 @@
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A74" s="6"/>
-      <c r="B74" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A74" s="13"/>
+      <c r="B74" s="3"/>
       <c r="C74" s="3"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="7"/>
-      <c r="F74" s="4"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="4"/>
-      <c r="M74" s="4"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+      <c r="M74" s="3"/>
+      <c r="N74" s="3"/>
+      <c r="O74" s="3"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="6"/>
-      <c r="B75" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A75" s="13"/>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A76" s="6"/>
-      <c r="B76" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A76" s="13"/>
+      <c r="B76" s="3"/>
       <c r="C76" s="3"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3"/>
+      <c r="K76" s="3"/>
+      <c r="L76" s="3"/>
+      <c r="M76" s="3"/>
+      <c r="N76" s="3"/>
+      <c r="O76" s="3"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="2"/>
-      <c r="B77" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A77" s="13"/>
+      <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+      <c r="H77" s="3"/>
+      <c r="I77" s="3"/>
+      <c r="J77" s="3"/>
+      <c r="K77" s="3"/>
+      <c r="L77" s="3"/>
+      <c r="M77" s="3"/>
+      <c r="N77" s="3"/>
+      <c r="O77" s="3"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A78" s="2"/>
-      <c r="B78" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A78" s="13"/>
+      <c r="B78" s="3"/>
       <c r="C78" s="3"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A79" s="13"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
-      <c r="D79" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -3210,22 +3217,16 @@
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
-      <c r="L79" s="3">
-        <v>8.1</v>
-      </c>
+      <c r="L79" s="3"/>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A80" s="13"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -3233,47 +3234,33 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="3">
-        <v>8.1999999999999993</v>
-      </c>
+      <c r="L80" s="3"/>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A81" s="13"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="3">
-        <v>17</v>
-      </c>
+      <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="3">
-        <v>8.3000000000000007</v>
-      </c>
+      <c r="L81" s="3"/>
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A82" s="13"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
-      <c r="D82" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -3281,207 +3268,157 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
-      <c r="L82" s="3">
-        <v>8.4</v>
-      </c>
+      <c r="L82" s="3"/>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A83" s="13"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="D83" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K83" s="3">
-        <v>17.3</v>
-      </c>
-      <c r="L83" s="3">
-        <v>7.1</v>
-      </c>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3">
-        <v>17.2</v>
-      </c>
-      <c r="L84" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="M84" s="3"/>
-      <c r="N84" s="3"/>
-      <c r="O84" s="3"/>
+      <c r="A84" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3">
-        <v>17</v>
-      </c>
-      <c r="L85" s="3">
-        <v>6</v>
-      </c>
-      <c r="M85" s="3"/>
-      <c r="N85" s="3"/>
-      <c r="O85" s="3"/>
+      <c r="A85" s="16"/>
+      <c r="B85" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="A86" s="14"/>
       <c r="B86" s="3" t="s">
-        <v>18</v>
+        <v>162</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="K86" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L86" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M86" s="3"/>
-      <c r="N86" s="3"/>
-      <c r="O86" s="3"/>
+        <v>163</v>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="K87" s="3">
-        <v>11.3</v>
-      </c>
-      <c r="L87" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M87" s="3"/>
-      <c r="N87" s="3"/>
-      <c r="O87" s="3"/>
+      <c r="A87" s="2"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="4"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="4"/>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-      <c r="J88" s="3">
-        <v>3.4</v>
-      </c>
-      <c r="K88" s="3">
-        <v>11.4</v>
-      </c>
-      <c r="L88" s="3">
-        <v>3.1</v>
-      </c>
-      <c r="M88" s="3"/>
-      <c r="N88" s="3"/>
-      <c r="O88" s="3"/>
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="4"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="4"/>
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D89" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E89" s="3"/>
-      <c r="F89" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
-      <c r="K89" s="3">
-        <v>11.7</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>49</v>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3">
+        <v>8.1</v>
       </c>
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
@@ -3489,90 +3426,70 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D90" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E90" s="3"/>
-      <c r="F90" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-      <c r="J90" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L90" s="3"/>
+      <c r="J90" s="3"/>
+      <c r="K90" s="3"/>
+      <c r="L90" s="3">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D91" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E91" s="3"/>
-      <c r="F91" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="3">
-        <v>4.3</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L91" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3">
+        <v>8.3000000000000007</v>
+      </c>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E92" s="3"/>
-      <c r="F92" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="K92" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L92" s="3" t="s">
-        <v>56</v>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3">
+        <v>8.4</v>
       </c>
       <c r="M92" s="3"/>
       <c r="N92" s="3"/>
@@ -3580,32 +3497,26 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E93" s="3"/>
-      <c r="F93" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K93" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L93" s="3" t="s">
-        <v>59</v>
+      <c r="J93" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K93" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="L93" s="3">
+        <v>7.1</v>
       </c>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -3613,28 +3524,24 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="E94" s="3"/>
-      <c r="F94" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="3" t="s">
-        <v>61</v>
+      <c r="K94" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="L94" s="3">
+        <v>6.4</v>
       </c>
       <c r="M94" s="3"/>
       <c r="N94" s="3"/>
@@ -3642,28 +3549,24 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D95" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E95" s="3"/>
-      <c r="F95" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3">
-        <v>10.5</v>
-      </c>
-      <c r="L95" s="3" t="s">
-        <v>63</v>
+        <v>17</v>
+      </c>
+      <c r="L95" s="3">
+        <v>6</v>
       </c>
       <c r="M95" s="3"/>
       <c r="N95" s="3"/>
@@ -3671,7 +3574,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>18</v>
@@ -3681,45 +3584,51 @@
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
+      <c r="F96" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3">
-        <v>12</v>
-      </c>
-      <c r="L96" s="3"/>
+      <c r="J96" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L96" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M96" s="3"/>
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D97" s="3"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
+      <c r="F97" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="3">
-        <v>13.3</v>
+        <v>3.4</v>
       </c>
       <c r="K97" s="3">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="L97" s="3" t="s">
-        <v>68</v>
+        <v>11.3</v>
+      </c>
+      <c r="L97" s="3">
+        <v>3.1</v>
       </c>
       <c r="M97" s="3"/>
       <c r="N97" s="3"/>
@@ -3727,49 +3636,59 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="3"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
+      <c r="F98" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="3">
-        <v>13.4</v>
-      </c>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="K98" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="L98" s="3">
+        <v>3.1</v>
+      </c>
       <c r="M98" s="3"/>
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B99" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C99" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F99" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3">
-        <v>9.1999999999999993</v>
+      <c r="K99" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="L99" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="M99" s="3"/>
       <c r="N99" s="3"/>
@@ -3777,109 +3696,152 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F100" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="K100" s="3"/>
-      <c r="L100" s="3" t="s">
-        <v>72</v>
-      </c>
+        <v>4.3</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L100" s="3"/>
       <c r="M100" s="3"/>
       <c r="N100" s="3"/>
       <c r="O100" s="3"/>
     </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L101" s="3"/>
+      <c r="M101" s="3"/>
+      <c r="N101" s="3"/>
+      <c r="O101" s="3"/>
+    </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C102" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="D102" s="3" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
+      <c r="F102" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
-      <c r="I102" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K102" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="L102" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="M102" s="3"/>
       <c r="N102" s="3"/>
       <c r="O102" s="3"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B103" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C103" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
+      <c r="F103" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="L103" s="3"/>
+      <c r="J103" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K103" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L103" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="M103" s="3"/>
       <c r="N103" s="3"/>
-      <c r="O103" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="O103" s="3"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
+      <c r="F104" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K104" s="3">
-        <v>16.3</v>
-      </c>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
       <c r="L104" s="3" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="M104" s="3"/>
       <c r="N104" s="3"/>
@@ -3887,30 +3849,28 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B105" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="C105" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="3">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="J105" s="3"/>
       <c r="K105" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L105" s="3">
-        <v>14.4</v>
+        <v>10.5</v>
+      </c>
+      <c r="L105" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="M105" s="3"/>
       <c r="N105" s="3"/>
@@ -3918,23 +3878,23 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-      <c r="J106" s="3">
-        <v>8.6999999999999993</v>
-      </c>
+      <c r="J106" s="3"/>
       <c r="K106" s="3">
-        <v>18.3</v>
+        <v>12</v>
       </c>
       <c r="L106" s="3"/>
       <c r="M106" s="3"/>
@@ -3943,12 +3903,16 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D107" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -3956,13 +3920,13 @@
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="3">
-        <v>8.8000000000000007</v>
+        <v>13.3</v>
       </c>
       <c r="K107" s="3">
-        <v>18.2</v>
-      </c>
-      <c r="L107" s="3">
-        <v>14.1</v>
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L107" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="M107" s="3"/>
       <c r="N107" s="3"/>
@@ -3970,12 +3934,12 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -3983,11 +3947,9 @@
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="3">
-        <v>15</v>
-      </c>
-      <c r="K108" s="3">
-        <v>18.399999999999999</v>
-      </c>
+        <v>13.4</v>
+      </c>
+      <c r="K108" s="3"/>
       <c r="L108" s="3"/>
       <c r="M108" s="3"/>
       <c r="N108" s="3"/>
@@ -3995,93 +3957,78 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
+      <c r="C109" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D109" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E109" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="3">
-        <v>16</v>
-      </c>
-      <c r="K109" s="3">
-        <v>18.5</v>
-      </c>
-      <c r="L109" s="3"/>
+      <c r="J109" s="3"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="M109" s="3"/>
       <c r="N109" s="3"/>
       <c r="O109" s="3"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E110" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
-      <c r="K110" s="3">
-        <v>19</v>
-      </c>
-      <c r="L110" s="3"/>
+      <c r="J110" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="M110" s="3"/>
       <c r="N110" s="3"/>
       <c r="O110" s="3"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3"/>
-      <c r="I111" s="3"/>
-      <c r="J111" s="3"/>
-      <c r="K111" s="3">
-        <v>19</v>
-      </c>
-      <c r="L111" s="3"/>
-      <c r="M111" s="3"/>
-      <c r="N111" s="3"/>
-      <c r="O111" s="3"/>
-    </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B112" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="B112" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C112" s="3"/>
       <c r="D112" s="3" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
-      <c r="I112" s="3"/>
+      <c r="I112" s="3">
+        <v>6.4</v>
+      </c>
       <c r="J112" s="3"/>
-      <c r="K112" s="3">
-        <v>19</v>
-      </c>
+      <c r="K112" s="3"/>
       <c r="L112" s="3"/>
       <c r="M112" s="3"/>
       <c r="N112" s="3"/>
@@ -4089,12 +4036,14 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
+      <c r="C113" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D113" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -4103,76 +4052,96 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3">
-        <v>19</v>
+        <v>16.2</v>
       </c>
       <c r="L113" s="3"/>
       <c r="M113" s="3"/>
       <c r="N113" s="3"/>
-      <c r="O113" s="3"/>
+      <c r="O113" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D114" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
+      <c r="J114" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="K114" s="3">
-        <v>19</v>
-      </c>
-      <c r="L114" s="3"/>
+        <v>16.3</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M114" s="3"/>
       <c r="N114" s="3"/>
       <c r="O114" s="3"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
+      <c r="C115" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D115" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
+      <c r="F115" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
-      <c r="J115" s="3"/>
+      <c r="J115" s="3">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K115" s="3">
-        <v>19</v>
-      </c>
-      <c r="L115" s="3"/>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L115" s="3">
+        <v>14.4</v>
+      </c>
       <c r="M115" s="3"/>
       <c r="N115" s="3"/>
       <c r="O115" s="3"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
-      <c r="J116" s="3"/>
+      <c r="J116" s="3">
+        <v>8.6999999999999993</v>
+      </c>
       <c r="K116" s="3">
-        <v>19</v>
+        <v>18.3</v>
       </c>
       <c r="L116" s="3"/>
       <c r="M116" s="3"/>
@@ -4181,14 +4150,12 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
@@ -4196,35 +4163,37 @@
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3">
-        <v>14.5</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K117" s="3">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="L117" s="3"/>
+        <v>18.2</v>
+      </c>
+      <c r="L117" s="3">
+        <v>14.1</v>
+      </c>
       <c r="M117" s="3"/>
       <c r="N117" s="3"/>
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
-      <c r="J118" s="3"/>
+      <c r="J118" s="3">
+        <v>15</v>
+      </c>
       <c r="K118" s="3">
-        <v>20.2</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="L118" s="3"/>
       <c r="M118" s="3"/>
@@ -4233,23 +4202,23 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-      <c r="J119" s="3"/>
+      <c r="J119" s="3">
+        <v>16</v>
+      </c>
       <c r="K119" s="3">
-        <v>20.3</v>
+        <v>18.5</v>
       </c>
       <c r="L119" s="3"/>
       <c r="M119" s="3"/>
@@ -4258,14 +4227,12 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
@@ -4274,7 +4241,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3">
-        <v>20.399999999999999</v>
+        <v>19</v>
       </c>
       <c r="L120" s="3"/>
       <c r="M120" s="3"/>
@@ -4283,14 +4250,12 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
@@ -4299,7 +4264,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="L121" s="3"/>
       <c r="M121" s="3"/>
@@ -4308,25 +4273,21 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E122" s="3"/>
       <c r="F122" s="3"/>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3">
-        <v>21.5</v>
+        <v>19</v>
       </c>
       <c r="L122" s="3"/>
       <c r="M122" s="3"/>
@@ -4335,25 +4296,21 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E123" s="3"/>
       <c r="F123" s="3"/>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3">
-        <v>21.4</v>
+        <v>19</v>
       </c>
       <c r="L123" s="3"/>
       <c r="M123" s="3"/>
@@ -4362,13 +4319,13 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B124" s="3"/>
       <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
       <c r="G124" s="3"/>
@@ -4376,31 +4333,31 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3">
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="L124" s="3"/>
-      <c r="M124" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="N124" s="3">
-        <v>6.8</v>
-      </c>
+      <c r="M124" s="3"/>
+      <c r="N124" s="3"/>
       <c r="O124" s="3"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
-      <c r="K125" s="3"/>
+      <c r="K125" s="3">
+        <v>19</v>
+      </c>
       <c r="L125" s="3"/>
       <c r="M125" s="3"/>
       <c r="N125" s="3"/>
@@ -4408,155 +4365,215 @@
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
+      <c r="D126" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
-      <c r="K126" s="3"/>
+      <c r="K126" s="3">
+        <v>19</v>
+      </c>
       <c r="L126" s="3"/>
-      <c r="M126" s="3">
-        <v>9</v>
-      </c>
+      <c r="M126" s="3"/>
       <c r="N126" s="3"/>
       <c r="O126" s="3"/>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B127" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
+      <c r="D127" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-      <c r="J127" s="3"/>
-      <c r="K127" s="3"/>
+      <c r="J127" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="K127" s="3">
+        <v>20.100000000000001</v>
+      </c>
       <c r="L127" s="3"/>
-      <c r="M127" s="3">
-        <v>10</v>
-      </c>
+      <c r="M127" s="3"/>
       <c r="N127" s="3"/>
       <c r="O127" s="3"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B128" s="3"/>
+        <v>98</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
-      <c r="K128" s="3"/>
+      <c r="K128" s="3">
+        <v>20.2</v>
+      </c>
       <c r="L128" s="3"/>
-      <c r="M128" s="3">
-        <v>10</v>
-      </c>
+      <c r="M128" s="3"/>
       <c r="N128" s="3"/>
       <c r="O128" s="3"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A129" s="3"/>
-      <c r="B129" s="3"/>
+      <c r="A129" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
+      <c r="D129" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
       <c r="G129" s="3"/>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
-      <c r="K129" s="3"/>
+      <c r="K129" s="3">
+        <v>20.3</v>
+      </c>
       <c r="L129" s="3"/>
       <c r="M129" s="3"/>
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A130" s="3"/>
-      <c r="B130" s="3"/>
+      <c r="A130" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
       <c r="G130" s="3"/>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
-      <c r="K130" s="3"/>
+      <c r="K130" s="3">
+        <v>20.399999999999999</v>
+      </c>
       <c r="L130" s="3"/>
       <c r="M130" s="3"/>
       <c r="N130" s="3"/>
       <c r="O130" s="3"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
+      <c r="A131" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
+      <c r="D131" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
-      <c r="K131" s="3"/>
+      <c r="K131" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L131" s="3"/>
       <c r="M131" s="3"/>
       <c r="N131" s="3"/>
       <c r="O131" s="3"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
+      <c r="A132" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
+      <c r="D132" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F132" s="3"/>
       <c r="G132" s="3"/>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
-      <c r="K132" s="3"/>
+      <c r="K132" s="3">
+        <v>21.5</v>
+      </c>
       <c r="L132" s="3"/>
       <c r="M132" s="3"/>
       <c r="N132" s="3"/>
       <c r="O132" s="3"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A133" s="3"/>
-      <c r="B133" s="3"/>
+      <c r="A133" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
+      <c r="D133" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
-      <c r="K133" s="3"/>
+      <c r="K133" s="3">
+        <v>21.4</v>
+      </c>
       <c r="L133" s="3"/>
       <c r="M133" s="3"/>
       <c r="N133" s="3"/>
       <c r="O133" s="3"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3"/>
+      <c r="A134" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
@@ -4565,14 +4582,22 @@
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
-      <c r="K134" s="3"/>
+      <c r="K134" s="3">
+        <v>20.5</v>
+      </c>
       <c r="L134" s="3"/>
-      <c r="M134" s="3"/>
-      <c r="N134" s="3"/>
+      <c r="M134" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="N134" s="3">
+        <v>6.8</v>
+      </c>
       <c r="O134" s="3"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A135" s="3"/>
+      <c r="A135" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
@@ -4589,7 +4614,9 @@
       <c r="O135" s="3"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A136" s="3"/>
+      <c r="A136" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
@@ -4601,22 +4628,197 @@
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
-      <c r="M136" s="3"/>
+      <c r="M136" s="3">
+        <v>9</v>
+      </c>
       <c r="N136" s="3"/>
       <c r="O136" s="3"/>
     </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+      <c r="E137" s="3"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="3"/>
+      <c r="I137" s="3"/>
+      <c r="J137" s="3"/>
+      <c r="K137" s="3"/>
+      <c r="L137" s="3"/>
+      <c r="M137" s="3">
+        <v>10</v>
+      </c>
+      <c r="N137" s="3"/>
+      <c r="O137" s="3"/>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="3"/>
+      <c r="L138" s="3"/>
+      <c r="M138" s="3">
+        <v>10</v>
+      </c>
+      <c r="N138" s="3"/>
+      <c r="O138" s="3"/>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+      <c r="E139" s="3"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="3"/>
+      <c r="I139" s="3"/>
+      <c r="J139" s="3"/>
+      <c r="K139" s="3"/>
+      <c r="L139" s="3"/>
+      <c r="M139" s="3"/>
+      <c r="N139" s="3"/>
+      <c r="O139" s="3"/>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="3"/>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="3"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="3"/>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+      <c r="E141" s="3"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="3"/>
+      <c r="I141" s="3"/>
+      <c r="J141" s="3"/>
+      <c r="K141" s="3"/>
+      <c r="L141" s="3"/>
+      <c r="M141" s="3"/>
+      <c r="N141" s="3"/>
+      <c r="O141" s="3"/>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="3"/>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="3"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="3"/>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+      <c r="E143" s="3"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="3"/>
+      <c r="I143" s="3"/>
+      <c r="J143" s="3"/>
+      <c r="K143" s="3"/>
+      <c r="L143" s="3"/>
+      <c r="M143" s="3"/>
+      <c r="N143" s="3"/>
+      <c r="O143" s="3"/>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="3"/>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="3"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="3"/>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+      <c r="E145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
+      <c r="O145" s="3"/>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+      <c r="E146" s="3"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="3"/>
+      <c r="I146" s="3"/>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3"/>
+      <c r="N146" s="3"/>
+      <c r="O146" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O135" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O136">
-    <sortCondition ref="H2:H136"/>
+  <autoFilter ref="A1:O145" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O146">
+    <sortCondition ref="H2:H146"/>
   </sortState>
-  <mergeCells count="13">
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A59:A61"/>
+  <mergeCells count="14">
+    <mergeCell ref="A84:A86"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A39"/>
     <mergeCell ref="A2:A4"/>
@@ -4624,13 +4826,19 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A59:A61"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:O2 A85:C95 E85:O90 E94:O95 F91:O93 D91:D93 A136 A5:O8 B3:O4 A79:O84 G8:G10 B9:F10 A11 A14 A96:O100 A102:O135 G9:O72 D11:F72 D74:O78 B11:B72 B74:B78 A73:O73">
+  <conditionalFormatting sqref="A2:O2 A95:C105 E95:O100 E104:O105 F101:O103 D101:D103 A146 A5:O8 B3:O4 A89:O94 G8:G10 B9:F10 A11 A14 A106:O110 A112:O145 G9:O72 D11:F72 B11:B72 B84:B88 A73:O83 D84:O88">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>$H2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:A31 A51:A53 A56 A59 A62:A68 A77:A78">
+  <conditionalFormatting sqref="A17:A31 A51:A53 A56 A59 A62:A68 A87:A88">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>$H17="Completed"</formula>
     </cfRule>

</xml_diff>

<commit_message>
docs: add table of content to K-Means chapter.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD35A8B-D160-D645-BA2F-F330C3E46D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66EB30E-606C-7847-B909-6F0E75F54C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$144</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="165">
   <si>
     <t>Topic</t>
   </si>
@@ -531,13 +531,16 @@
   </si>
   <si>
     <t>Vector Semantics and Embeddings</t>
+  </si>
+  <si>
+    <t>https://goodboychan.github.io/python/datacamp/statistics/2020/08/28/01-More-Distributions-and-the-Central-Limit-Theorem.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,6 +551,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -640,10 +651,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -662,6 +674,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -671,20 +695,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
@@ -1128,11 +1142,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845021A4-9E60-AD4D-9E49-75BA82CC8B8F}">
-  <dimension ref="A1:O146"/>
+  <dimension ref="A1:O145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84:H86"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1199,7 +1213,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1238,7 +1252,7 @@
       <c r="O2" s="2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1259,7 +1273,7 @@
       <c r="O3" s="2"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1365,7 +1379,7 @@
       <c r="O7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1400,7 +1414,7 @@
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>30</v>
@@ -1425,7 +1439,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>30</v>
@@ -1450,7 +1464,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1475,7 +1489,7 @@
       <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>123</v>
       </c>
@@ -1498,7 +1512,7 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="4" t="s">
         <v>123</v>
       </c>
@@ -1521,7 +1535,7 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1546,7 +1560,7 @@
       <c r="O14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3" t="s">
         <v>120</v>
       </c>
@@ -1569,7 +1583,7 @@
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="4" t="s">
         <v>120</v>
       </c>
@@ -1966,7 +1980,7 @@
       <c r="O30" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1995,7 +2009,7 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="11"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>22</v>
       </c>
@@ -2022,7 +2036,7 @@
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="3" t="s">
         <v>22</v>
       </c>
@@ -2049,7 +2063,7 @@
       <c r="O33" s="4"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2078,7 +2092,7 @@
       <c r="O34" s="4"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
@@ -2105,7 +2119,7 @@
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
@@ -2132,7 +2146,7 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="14" t="s">
         <v>141</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2161,7 +2175,7 @@
       <c r="O37" s="4"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="11"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
@@ -2188,7 +2202,7 @@
       <c r="O38" s="4"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="3" t="s">
         <v>22</v>
       </c>
@@ -2215,7 +2229,7 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="14" t="s">
         <v>142</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2244,7 +2258,7 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A41" s="11"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="4" t="s">
         <v>22</v>
       </c>
@@ -2271,7 +2285,7 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A42" s="12"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="3" t="s">
         <v>22</v>
       </c>
@@ -2298,7 +2312,7 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="14" t="s">
         <v>143</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2327,7 +2341,7 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="4" t="s">
         <v>22</v>
       </c>
@@ -2354,7 +2368,7 @@
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A45" s="12"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="4" t="s">
         <v>22</v>
       </c>
@@ -2566,7 +2580,7 @@
       <c r="O52" s="4"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="14" t="s">
         <v>147</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2595,7 +2609,7 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="3" t="s">
         <v>22</v>
       </c>
@@ -2622,7 +2636,7 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="3" t="s">
         <v>22</v>
       </c>
@@ -2649,7 +2663,7 @@
       <c r="O55" s="4"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
+      <c r="A56" s="14" t="s">
         <v>148</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2678,7 +2692,7 @@
       <c r="O56" s="4"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="11"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="4" t="s">
         <v>22</v>
       </c>
@@ -2705,7 +2719,7 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="12"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="4" t="s">
         <v>22</v>
       </c>
@@ -2732,7 +2746,7 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="14" t="s">
         <v>149</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -2761,7 +2775,7 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="11"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="4" t="s">
         <v>22</v>
       </c>
@@ -2788,7 +2802,7 @@
       <c r="O60" s="4"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="12"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="4" t="s">
         <v>22</v>
       </c>
@@ -2965,7 +2979,7 @@
       <c r="O67" s="4"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="14" t="s">
         <v>158</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -2994,7 +3008,7 @@
       <c r="O68" s="4"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="11"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="4" t="s">
         <v>22</v>
       </c>
@@ -3021,7 +3035,7 @@
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="12"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="3" t="s">
         <v>22</v>
       </c>
@@ -3121,7 +3135,7 @@
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A74" s="13"/>
+      <c r="A74" s="10"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -3138,7 +3152,7 @@
       <c r="O74" s="3"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="13"/>
+      <c r="A75" s="10"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -3155,7 +3169,7 @@
       <c r="O75" s="3"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
+      <c r="A76" s="10"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -3172,7 +3186,7 @@
       <c r="O76" s="3"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="13"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -3189,7 +3203,7 @@
       <c r="O77" s="3"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A78" s="13"/>
+      <c r="A78" s="10"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -3206,7 +3220,7 @@
       <c r="O78" s="3"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A79" s="13"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -3223,7 +3237,7 @@
       <c r="O79" s="3"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A80" s="13"/>
+      <c r="A80" s="10"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -3240,7 +3254,7 @@
       <c r="O80" s="3"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A81" s="13"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -3257,7 +3271,7 @@
       <c r="O81" s="3"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A82" s="13"/>
+      <c r="A82" s="10"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -3274,7 +3288,7 @@
       <c r="O82" s="3"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A83" s="13"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -3291,7 +3305,7 @@
       <c r="O83" s="3"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="11" t="s">
         <v>161</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -3318,7 +3332,7 @@
       <c r="O84" s="4"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A85" s="16"/>
+      <c r="A85" s="12"/>
       <c r="B85" s="3" t="s">
         <v>162</v>
       </c>
@@ -3343,7 +3357,7 @@
       <c r="O85" s="4"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="3" t="s">
         <v>162</v>
       </c>
@@ -4009,84 +4023,117 @@
       <c r="N110" s="3"/>
       <c r="O110" s="3"/>
     </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3">
+        <v>6.4</v>
+      </c>
+      <c r="J111" s="3"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+      <c r="M111" s="3"/>
+      <c r="N111" s="3"/>
+      <c r="O111" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C112" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="D112" s="3" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
-      <c r="I112" s="3">
-        <v>6.4</v>
-      </c>
+      <c r="I112" s="3"/>
       <c r="J112" s="3"/>
-      <c r="K112" s="3"/>
+      <c r="K112" s="3">
+        <v>16.2</v>
+      </c>
       <c r="L112" s="3"/>
       <c r="M112" s="3"/>
       <c r="N112" s="3"/>
-      <c r="O112" s="3"/>
+      <c r="O112" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B113" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C113" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
-      <c r="J113" s="3"/>
+      <c r="J113" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="K113" s="3">
-        <v>16.2</v>
-      </c>
-      <c r="L113" s="3"/>
+        <v>16.3</v>
+      </c>
+      <c r="L113" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M113" s="3"/>
       <c r="N113" s="3"/>
-      <c r="O113" s="3" t="s">
-        <v>77</v>
-      </c>
+      <c r="O113" s="3"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B114" s="3"/>
       <c r="C114" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
+      <c r="F114" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
-      <c r="J114" s="3" t="s">
-        <v>79</v>
+      <c r="J114" s="3">
+        <v>9.1999999999999993</v>
       </c>
       <c r="K114" s="3">
-        <v>16.3</v>
-      </c>
-      <c r="L114" s="3" t="s">
-        <v>80</v>
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L114" s="3">
+        <v>14.4</v>
       </c>
       <c r="M114" s="3"/>
       <c r="N114" s="3"/>
@@ -4094,38 +4141,32 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B115" s="3"/>
-      <c r="C115" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="C115" s="3"/>
       <c r="D115" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E115" s="3"/>
-      <c r="F115" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="3">
-        <v>9.1999999999999993</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="K115" s="3">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="L115" s="3">
-        <v>14.4</v>
-      </c>
+        <v>18.3</v>
+      </c>
+      <c r="L115" s="3"/>
       <c r="M115" s="3"/>
       <c r="N115" s="3"/>
       <c r="O115" s="3"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -4138,19 +4179,21 @@
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
       <c r="J116" s="3">
-        <v>8.6999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K116" s="3">
-        <v>18.3</v>
-      </c>
-      <c r="L116" s="3"/>
+        <v>18.2</v>
+      </c>
+      <c r="L116" s="3">
+        <v>14.1</v>
+      </c>
       <c r="M116" s="3"/>
       <c r="N116" s="3"/>
       <c r="O116" s="3"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -4163,21 +4206,19 @@
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="3">
-        <v>8.8000000000000007</v>
+        <v>15</v>
       </c>
       <c r="K117" s="3">
-        <v>18.2</v>
-      </c>
-      <c r="L117" s="3">
-        <v>14.1</v>
-      </c>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="L117" s="3"/>
       <c r="M117" s="3"/>
       <c r="N117" s="3"/>
       <c r="O117" s="3"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -4190,10 +4231,10 @@
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K118" s="3">
-        <v>18.399999999999999</v>
+        <v>18.5</v>
       </c>
       <c r="L118" s="3"/>
       <c r="M118" s="3"/>
@@ -4202,23 +4243,21 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
-      <c r="J119" s="3">
-        <v>16</v>
-      </c>
+      <c r="J119" s="3"/>
       <c r="K119" s="3">
-        <v>18.5</v>
+        <v>19</v>
       </c>
       <c r="L119" s="3"/>
       <c r="M119" s="3"/>
@@ -4227,7 +4266,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -4250,7 +4289,7 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -4273,7 +4312,7 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -4296,7 +4335,7 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -4319,7 +4358,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -4342,7 +4381,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -4365,21 +4404,25 @@
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B126" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
-      <c r="J126" s="3"/>
+      <c r="J126" s="3">
+        <v>14.5</v>
+      </c>
       <c r="K126" s="3">
-        <v>19</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L126" s="3"/>
       <c r="M126" s="3"/>
@@ -4388,7 +4431,7 @@
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B127" s="3" t="s">
         <v>32</v>
@@ -4402,11 +4445,9 @@
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
-      <c r="J127" s="3">
-        <v>14.5</v>
-      </c>
+      <c r="J127" s="3"/>
       <c r="K127" s="3">
-        <v>20.100000000000001</v>
+        <v>20.2</v>
       </c>
       <c r="L127" s="3"/>
       <c r="M127" s="3"/>
@@ -4415,7 +4456,7 @@
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B128" s="3" t="s">
         <v>32</v>
@@ -4431,7 +4472,7 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3">
-        <v>20.2</v>
+        <v>20.3</v>
       </c>
       <c r="L128" s="3"/>
       <c r="M128" s="3"/>
@@ -4440,7 +4481,7 @@
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B129" s="3" t="s">
         <v>32</v>
@@ -4456,7 +4497,7 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3">
-        <v>20.3</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="L129" s="3"/>
       <c r="M129" s="3"/>
@@ -4465,7 +4506,7 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B130" s="3" t="s">
         <v>32</v>
@@ -4481,7 +4522,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3">
-        <v>20.399999999999999</v>
+        <v>20.5</v>
       </c>
       <c r="L130" s="3"/>
       <c r="M130" s="3"/>
@@ -4490,23 +4531,25 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C131" s="3"/>
       <c r="D131" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E131" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="F131" s="3"/>
       <c r="G131" s="3"/>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3">
-        <v>20.5</v>
+        <v>21.5</v>
       </c>
       <c r="L131" s="3"/>
       <c r="M131" s="3"/>
@@ -4515,7 +4558,7 @@
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B132" s="3" t="s">
         <v>32</v>
@@ -4533,7 +4576,7 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3">
-        <v>21.5</v>
+        <v>21.4</v>
       </c>
       <c r="L132" s="3"/>
       <c r="M132" s="3"/>
@@ -4542,38 +4585,36 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="C133" s="3"/>
-      <c r="D133" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E133" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="D133" s="3"/>
+      <c r="E133" s="3"/>
       <c r="F133" s="3"/>
       <c r="G133" s="3"/>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3">
-        <v>21.4</v>
+        <v>20.5</v>
       </c>
       <c r="L133" s="3"/>
-      <c r="M133" s="3"/>
-      <c r="N133" s="3"/>
+      <c r="M133" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="N133" s="3">
+        <v>6.8</v>
+      </c>
       <c r="O133" s="3"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>104</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
@@ -4582,21 +4623,15 @@
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
-      <c r="K134" s="3">
-        <v>20.5</v>
-      </c>
+      <c r="K134" s="3"/>
       <c r="L134" s="3"/>
-      <c r="M134" s="3">
-        <v>15.1</v>
-      </c>
-      <c r="N134" s="3">
-        <v>6.8</v>
-      </c>
+      <c r="M134" s="3"/>
+      <c r="N134" s="3"/>
       <c r="O134" s="3"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -4609,13 +4644,15 @@
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
       <c r="L135" s="3"/>
-      <c r="M135" s="3"/>
+      <c r="M135" s="3">
+        <v>9</v>
+      </c>
       <c r="N135" s="3"/>
       <c r="O135" s="3"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -4629,14 +4666,14 @@
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
       <c r="M136" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N136" s="3"/>
       <c r="O136" s="3"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -4656,9 +4693,7 @@
       <c r="O137" s="3"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>108</v>
-      </c>
+      <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
@@ -4670,9 +4705,7 @@
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
       <c r="L138" s="3"/>
-      <c r="M138" s="3">
-        <v>10</v>
-      </c>
+      <c r="M138" s="3"/>
       <c r="N138" s="3"/>
       <c r="O138" s="3"/>
     </row>
@@ -4795,27 +4828,10 @@
       <c r="N145" s="3"/>
       <c r="O145" s="3"/>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A146" s="3"/>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
-      <c r="E146" s="3"/>
-      <c r="F146" s="3"/>
-      <c r="G146" s="3"/>
-      <c r="H146" s="3"/>
-      <c r="I146" s="3"/>
-      <c r="J146" s="3"/>
-      <c r="K146" s="3"/>
-      <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
-      <c r="N146" s="3"/>
-      <c r="O146" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:O145" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O146">
-    <sortCondition ref="H2:H146"/>
+  <autoFilter ref="A1:O144" xr:uid="{17BC1D5B-D4A2-A141-B90E-034529CBCDEB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O145">
+    <sortCondition ref="H2:H145"/>
   </sortState>
   <mergeCells count="14">
     <mergeCell ref="A84:A86"/>
@@ -4833,7 +4849,7 @@
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="A59:A61"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:O2 A95:C105 E95:O100 E104:O105 F101:O103 D101:D103 A146 A5:O8 B3:O4 A89:O94 G8:G10 B9:F10 A11 A14 A106:O110 A112:O145 G9:O72 D11:F72 B11:B72 B84:B88 A73:O83 D84:O88">
+  <conditionalFormatting sqref="A2:O2 A95:C105 E95:O100 E104:O105 F101:O103 D101:D103 A145 A5:O8 B3:O4 A89:O94 G8:G10 B9:F10 A11 A14 A106:O144 G9:O72 D11:F72 B11:B72 B84:B88 A73:O83 D84:O88">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>$H2="Completed"</formula>
     </cfRule>
@@ -4898,6 +4914,9 @@
       <formula>$H34="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="O111" r:id="rId1" xr:uid="{8FF4790D-4F20-1449-805A-F347E94F78EB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: update content on K-Means and linear regression.
</commit_message>
<xml_diff>
--- a/galaxy/references_resources_roadmap/roadmap.xlsx
+++ b/galaxy/references_resources_roadmap/roadmap.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaohn/gao/gaohn-galaxy/galaxy/references_resources_roadmap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66EB30E-606C-7847-B909-6F0E75F54C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2739D18D-E3CD-4A48-A7A9-4D47A0D3F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50400" yWindow="3860" windowWidth="38400" windowHeight="21100" xr2:uid="{0BF26694-6EBC-134A-B08D-954D18280C10}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Todos!$A$1:$O$144</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="166">
   <si>
     <t>Topic</t>
   </si>
@@ -534,6 +535,9 @@
   </si>
   <si>
     <t>https://goodboychan.github.io/python/datacamp/statistics/2020/08/28/01-More-Distributions-and-the-Central-Limit-Theorem.html</t>
+  </si>
+  <si>
+    <t>Start with ISLR since they have exercises and solutions, but reference book use Kevin Murphy's book.</t>
   </si>
 </sst>
 </file>
@@ -1145,8 +1149,8 @@
   <dimension ref="A1:O145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3603,7 +3607,9 @@
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
+      <c r="I96" s="3">
+        <v>7.1</v>
+      </c>
       <c r="J96" s="3">
         <v>3.2</v>
       </c>
@@ -4919,4 +4925,24 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B5CF0F-6ABB-8E4D-8B6B-5CFC6C99D1AF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>